<commit_message>
Pairwise sensitivity models added.
</commit_message>
<xml_diff>
--- a/data/studies_data.xlsx
+++ b/data/studies_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Steele Research Ltd\Stronger by Science\pcos_ree_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A155659-82D5-45D2-A84D-B90EAE97303B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8376398-A129-4026-94FA-643CB2277A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="159">
   <si>
     <t>study</t>
   </si>
@@ -954,10 +954,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE7CBA6-16D3-4F56-AAFF-D7A43475C68F}">
   <dimension ref="A1:AY39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="AC16" sqref="AC16"/>
+      <selection pane="bottomLeft" activeCell="Z39" sqref="Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1180,9 @@
       <c r="Y2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="Z2" s="6"/>
+      <c r="Z2" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="AA2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1261,7 +1263,9 @@
       <c r="Y3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="Z3" s="7"/>
+      <c r="Z3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1336,7 +1340,9 @@
       <c r="Y4" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="Z4" s="7"/>
+      <c r="Z4" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA4" s="4" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1411,9 @@
       <c r="Y5" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="Z5" s="7"/>
+      <c r="Z5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA5" s="4" t="s">
         <v>25</v>
       </c>
@@ -1474,7 +1482,9 @@
       <c r="Y6" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Z6" s="7"/>
+      <c r="Z6" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1543,7 +1553,9 @@
       <c r="Y7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="Z7" s="7"/>
+      <c r="Z7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA7" s="4" t="s">
         <v>25</v>
       </c>
@@ -1700,7 +1712,9 @@
       <c r="Y9" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="Z9" s="7"/>
+      <c r="Z9" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA9" s="4" t="s">
         <v>60</v>
       </c>
@@ -2185,7 +2199,9 @@
       <c r="Y15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="Z15" s="7"/>
+      <c r="Z15" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA15" s="4" t="s">
         <v>25</v>
       </c>
@@ -2277,7 +2293,9 @@
       <c r="Y16" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="Z16" s="7"/>
+      <c r="Z16" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA16" s="4" t="s">
         <v>25</v>
       </c>
@@ -2744,7 +2762,9 @@
       <c r="Y26" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="Z26" s="7"/>
+      <c r="Z26" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA26" s="4" t="s">
         <v>25</v>
       </c>
@@ -2807,7 +2827,9 @@
       <c r="Y27" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="Z27" s="7"/>
+      <c r="Z27" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA27" s="4" t="s">
         <v>25</v>
       </c>
@@ -3062,7 +3084,9 @@
       <c r="Y30" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="Z30" s="7"/>
+      <c r="Z30" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA30" s="4" t="s">
         <v>25</v>
       </c>
@@ -3144,7 +3168,9 @@
       <c r="Y31" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="Z31" s="7"/>
+      <c r="Z31" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA31" s="4" t="s">
         <v>25</v>
       </c>
@@ -3226,7 +3252,9 @@
       <c r="Y32" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Z32" s="7"/>
+      <c r="Z32" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA32" s="4" t="s">
         <v>25</v>
       </c>
@@ -3304,7 +3332,9 @@
       <c r="Y33" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="Z33" s="7"/>
+      <c r="Z33" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA33" s="4" t="s">
         <v>25</v>
       </c>
@@ -3379,7 +3409,9 @@
       <c r="Y34" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="Z34" s="7"/>
+      <c r="Z34" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA34" s="4" t="s">
         <v>25</v>
       </c>
@@ -3454,7 +3486,9 @@
       <c r="Y35" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="Z35" s="7"/>
+      <c r="Z35" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA35" s="4" t="s">
         <v>25</v>
       </c>
@@ -3529,7 +3563,9 @@
       <c r="Y36" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="Z36" s="7"/>
+      <c r="Z36" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA36" s="4" t="s">
         <v>25</v>
       </c>
@@ -3613,7 +3649,9 @@
       <c r="Y37" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="Z37" s="7"/>
+      <c r="Z37" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA37" s="4" t="s">
         <v>25</v>
       </c>
@@ -3697,7 +3735,9 @@
       <c r="Y38" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="Z38" s="7"/>
+      <c r="Z38" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA38" s="4" t="s">
         <v>25</v>
       </c>
@@ -3781,7 +3821,9 @@
       <c r="Y39" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="Z39" s="7"/>
+      <c r="Z39" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="AA39" s="4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Added to pipeline esitmation of missing BMIs, heights, weights.
</commit_message>
<xml_diff>
--- a/data/studies_data.xlsx
+++ b/data/studies_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Steele Research Ltd\Stronger by Science\pcos_ree_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8376398-A129-4026-94FA-643CB2277A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEEB213-381C-4852-B700-7D2A9B1554DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
+    <workbookView xWindow="4950" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="159">
   <si>
     <t>study</t>
   </si>
@@ -318,9 +318,6 @@
   </si>
   <si>
     <t>post_intervention</t>
-  </si>
-  <si>
-    <t>Hyperinsulinemic–euglycemic clamp technique, M-value (mg/kg_FFM x min) = 9.8 (SD = 3.7), 72.5% classified as IR based on cut off value of 11.76, Fasting glucose (mg/dL) = 85.3 (SD = 9.5), Fasting insulin (mU/L) = 16.2 (SD = 12.6)</t>
   </si>
   <si>
     <t>Fasting glucose (mg/dL) = 83.4 (SD = 5.9), Fasting insulin (mU/L) = 7 (SD = 5)</t>
@@ -420,15 +417,6 @@
     <t>Engaged in sporting activities &lt; 2 days/week - 80%</t>
   </si>
   <si>
-    <t>Hyperinsulinemic–euglycemic clamp technique, M-value (mg/kg/min, median) = 6.6 (IQR = 5.5-7.3)</t>
-  </si>
-  <si>
-    <t>Hyperinsulinemic–euglycemic clamp technique, M-value -(mg/kg/min, median) = 9.1 (IQR  7.7-10)</t>
-  </si>
-  <si>
-    <t>Hyperinsulinemic–euglycemic clamp technique, M-value (mg/kg/min, median) = 11.9 (IQR = 9.4-14.5)</t>
-  </si>
-  <si>
     <t>White/Caucasian = 6, Hispanic = 3, Native American = 1</t>
   </si>
   <si>
@@ -515,6 +503,18 @@
   </si>
   <si>
     <t>kcal/kg</t>
+  </si>
+  <si>
+    <t>Hyperinsulinemic euglycemic clamp technique, M-value (mg/kg_FFM x min) = 9.8 (SD = 3.7), 72.5% classified as IR based on cut off value of 11.76, Fasting glucose (mg/dL) = 85.3 (SD = 9.5), Fasting insulin (mU/L) = 16.2 (SD = 12.6)</t>
+  </si>
+  <si>
+    <t>Hyperinsulinemic euglycemic clamp technique, M-value (mg/kg/min, median) = 6.6 (IQR = 5.5-7.3)</t>
+  </si>
+  <si>
+    <t>Hyperinsulinemic euglycemic clamp technique, M-value -(mg/kg/min, median) = 9.1 (IQR  7.7-10)</t>
+  </si>
+  <si>
+    <t>Hyperinsulinemic euglycemic clamp technique, M-value (mg/kg/min, median) = 11.9 (IQR = 9.4-14.5)</t>
   </si>
 </sst>
 </file>
@@ -954,10 +954,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE7CBA6-16D3-4F56-AAFF-D7A43475C68F}">
   <dimension ref="A1:AY39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Z39" sqref="Z39"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,40 +996,40 @@
         <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>51</v>
@@ -1041,10 +1041,10 @@
         <v>53</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>24</v>
@@ -1089,10 +1089,10 @@
         <v>48</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>68</v>
@@ -1110,10 +1110,10 @@
         <v>50</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>71</v>
@@ -1178,7 +1178,7 @@
         <v>54</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="Z2" s="6" t="s">
         <v>38</v>
@@ -1261,7 +1261,7 @@
         <v>54</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z3" s="7" t="s">
         <v>2</v>
@@ -1329,16 +1329,16 @@
         <v>6.4</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>56</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z4" s="7" t="s">
         <v>38</v>
@@ -1400,16 +1400,16 @@
         <v>5.8</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>56</v>
       </c>
       <c r="Y5" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z5" s="7" t="s">
         <v>2</v>
@@ -1471,16 +1471,16 @@
         <v>5.6</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z6" s="7" t="s">
         <v>38</v>
@@ -1542,16 +1542,16 @@
         <v>5.7</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>56</v>
       </c>
       <c r="Y7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z7" s="7" t="s">
         <v>2</v>
@@ -1619,7 +1619,7 @@
         <v>3.7</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>56</v>
@@ -1701,16 +1701,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>59</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z9" s="7" t="s">
         <v>38</v>
@@ -1784,16 +1784,16 @@
         <v>3.6</v>
       </c>
       <c r="V10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="AA10" s="2" t="s">
         <v>25</v>
@@ -1812,7 +1812,7 @@
         <v>245</v>
       </c>
       <c r="AY10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:51" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1868,16 +1868,16 @@
         <v>3</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="AA11" s="2" t="s">
         <v>25</v>
@@ -1896,7 +1896,7 @@
         <v>181</v>
       </c>
       <c r="AY11" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:51" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1952,16 +1952,16 @@
         <v>3.6</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="AA12" s="2" t="s">
         <v>25</v>
@@ -1980,7 +1980,7 @@
         <v>259</v>
       </c>
       <c r="AY12" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:51" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -2188,10 +2188,10 @@
         <v>4.2</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>59</v>
@@ -2209,7 +2209,7 @@
         <v>10</v>
       </c>
       <c r="AC15" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AK15" s="4">
         <f>0.21*2*24</f>
@@ -2282,10 +2282,10 @@
         <v>4.5</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>59</v>
@@ -2303,7 +2303,7 @@
         <v>10</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AK16" s="4">
         <f>0.21*2*24</f>
@@ -2342,6 +2342,9 @@
       <c r="H17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I17" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J17" s="2">
         <v>23.56</v>
       </c>
@@ -2389,6 +2392,9 @@
       <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I18" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J18" s="2">
         <v>23.97</v>
       </c>
@@ -2436,6 +2442,9 @@
       <c r="H19" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="I19" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J19" s="2">
         <v>25.17</v>
       </c>
@@ -2483,6 +2492,9 @@
       <c r="H20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I20" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J20" s="2">
         <v>23.98</v>
       </c>
@@ -2524,6 +2536,9 @@
       <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="I21" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J21" s="2">
         <v>27</v>
       </c>
@@ -2565,6 +2580,9 @@
       <c r="H22" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="I22" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J22" s="2">
         <v>34</v>
       </c>
@@ -2606,6 +2624,9 @@
       <c r="H23" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I23" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J23" s="2">
         <v>24</v>
       </c>
@@ -2653,6 +2674,9 @@
       <c r="H24" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I24" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J24" s="2">
         <v>22.82</v>
       </c>
@@ -2697,6 +2721,9 @@
       <c r="H25" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="I25" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="J25" s="2">
         <v>22.91</v>
       </c>
@@ -2760,7 +2787,7 @@
         <v>74</v>
       </c>
       <c r="Y26" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="Z26" s="7" t="s">
         <v>38</v>
@@ -2825,7 +2852,7 @@
         <v>74</v>
       </c>
       <c r="Y27" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Z27" s="7" t="s">
         <v>2</v>
@@ -2903,13 +2930,13 @@
         <v>3.3625000000000003</v>
       </c>
       <c r="V28" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="X28" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Z28" s="7"/>
       <c r="AA28" s="4" t="s">
@@ -2931,7 +2958,7 @@
         <v>7774</v>
       </c>
       <c r="AY28" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -2991,13 +3018,13 @@
         <v>2.4999999999999996</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="X29" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Y29" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="Z29" s="7"/>
       <c r="AA29" s="4" t="s">
@@ -3019,7 +3046,7 @@
         <v>8492</v>
       </c>
       <c r="AY29" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:51" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -3324,13 +3351,13 @@
         <v>5.2915026221291814</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>79</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="Z33" s="7" t="s">
         <v>38</v>
@@ -3401,13 +3428,13 @@
         <v>5.8206528843420999</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="X34" s="4" t="s">
         <v>79</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Z34" s="7" t="s">
         <v>2</v>
@@ -3478,13 +3505,13 @@
         <v>7.6026311234992852</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="X35" s="4" t="s">
         <v>79</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Z35" s="7" t="s">
         <v>38</v>
@@ -3555,13 +3582,13 @@
         <v>6.7082039324993694</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>79</v>
       </c>
       <c r="Y36" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="Z36" s="7" t="s">
         <v>38</v>
@@ -3638,16 +3665,16 @@
         <v>12.244998979175133</v>
       </c>
       <c r="V37" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="W37" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="X37" s="4" t="s">
         <v>81</v>
       </c>
       <c r="Y37" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Z37" s="7" t="s">
         <v>38</v>
@@ -3694,7 +3721,7 @@
         <v>22</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J38" s="4">
         <v>32.1</v>
@@ -3724,16 +3751,16 @@
         <v>11.07880860020607</v>
       </c>
       <c r="V38" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="W38" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="X38" s="4" t="s">
         <v>81</v>
       </c>
       <c r="Y38" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Z38" s="7" t="s">
         <v>38</v>
@@ -3810,16 +3837,16 @@
         <v>11.989578808281799</v>
       </c>
       <c r="V39" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="W39" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="X39" s="4" t="s">
         <v>81</v>
       </c>
       <c r="Y39" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="Z39" s="7" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Updated demographics table functions for systematic review results.
</commit_message>
<xml_diff>
--- a/data/studies_data.xlsx
+++ b/data/studies_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Steele Research Ltd\Stronger by Science\pcos_ree_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEEB213-381C-4852-B700-7D2A9B1554DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A7C9AF-AE33-4372-9019-1C9340A58305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,12 +558,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,10 +606,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -954,10 +945,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE7CBA6-16D3-4F56-AAFF-D7A43475C68F}">
   <dimension ref="A1:AY39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,10 +1251,10 @@
       <c r="X3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Y3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="Z3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="AA3" s="4" t="s">
@@ -1337,10 +1328,10 @@
       <c r="X4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="7" t="s">
+      <c r="Y4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA4" s="4" t="s">
@@ -1408,10 +1399,10 @@
       <c r="X5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y5" s="7" t="s">
+      <c r="Y5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="Z5" s="7" t="s">
+      <c r="Z5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="AA5" s="4" t="s">
@@ -1479,10 +1470,10 @@
       <c r="X6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y6" s="7" t="s">
+      <c r="Y6" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="Z6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA6" s="4" t="s">
@@ -1550,10 +1541,10 @@
       <c r="X7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y7" s="7" t="s">
+      <c r="Y7" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="Z7" s="7" t="s">
+      <c r="Z7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="AA7" s="4" t="s">
@@ -1624,8 +1615,6 @@
       <c r="X8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
       <c r="AA8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1709,10 +1698,10 @@
       <c r="X9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="7" t="s">
+      <c r="Y9" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="Z9" s="7" t="s">
+      <c r="Z9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA9" s="4" t="s">
@@ -1731,255 +1720,273 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="5">
         <v>2016</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="4">
         <v>26</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="4">
         <v>5.2</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="4">
         <v>41.2</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="4">
         <v>12.5</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="4">
         <v>56.3</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10" s="4">
         <v>5</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="4">
         <v>34.1</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="4">
         <v>3.6</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="V10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Y10" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AA10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB10" s="2">
+      <c r="AA10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB10" s="4">
         <v>6</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AC10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AL10" s="2">
+      <c r="AE10" s="4">
         <v>1411</v>
       </c>
-      <c r="AQ10" s="2">
+      <c r="AJ10" s="4">
+        <v>245</v>
+      </c>
+      <c r="AL10" s="4">
+        <v>1411</v>
+      </c>
+      <c r="AQ10" s="4">
         <f>1613-1368</f>
         <v>245</v>
       </c>
-      <c r="AY10" s="2" t="s">
+      <c r="AY10" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>6</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="5">
         <v>2016</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="4">
         <v>27</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="4">
         <v>3.7</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="4">
         <v>23.3</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="4">
         <v>6.9</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="4">
         <v>47.4</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="4">
         <v>5.6</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="4">
         <v>26.4</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="4">
         <v>3</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="V11" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="W11" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="X11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Y11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="AA11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB11" s="2">
+      <c r="AA11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB11" s="4">
         <v>8</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AC11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AL11" s="2">
+      <c r="AE11" s="4">
         <v>1274</v>
       </c>
-      <c r="AQ11" s="2">
+      <c r="AJ11" s="4">
+        <v>181</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>1274</v>
+      </c>
+      <c r="AQ11" s="4">
         <f>1355-1174</f>
         <v>181</v>
       </c>
-      <c r="AY11" s="2" t="s">
+      <c r="AY11" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:51" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="5">
         <v>2016</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="4">
         <v>23</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="4">
         <v>0.7</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="4">
         <v>17.100000000000001</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="4">
         <v>7.6</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="4">
         <v>45.9</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="4">
         <v>6.7</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="4">
         <v>22.5</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="4">
         <v>3.6</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="V12" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="W12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="X12" s="2" t="s">
+      <c r="X12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Y12" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AA12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB12" s="2">
+      <c r="AA12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB12" s="4">
         <v>10</v>
       </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AC12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AL12" s="2">
+      <c r="AE12" s="4">
         <v>1239</v>
       </c>
-      <c r="AQ12" s="2">
+      <c r="AJ12" s="4">
+        <v>259</v>
+      </c>
+      <c r="AL12" s="4">
+        <v>1239</v>
+      </c>
+      <c r="AQ12" s="4">
         <f>1454-1195</f>
         <v>259</v>
       </c>
-      <c r="AY12" s="2" t="s">
+      <c r="AY12" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2038,8 +2045,6 @@
       <c r="X13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
       <c r="AA13" s="4" t="s">
         <v>25</v>
       </c>
@@ -2111,8 +2116,6 @@
       <c r="X14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
       <c r="AA14" s="4" t="s">
         <v>25</v>
       </c>
@@ -2196,10 +2199,10 @@
       <c r="X15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y15" s="7" t="s">
+      <c r="Y15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Z15" s="7" t="s">
+      <c r="Z15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA15" s="4" t="s">
@@ -2290,10 +2293,10 @@
       <c r="X16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y16" s="7" t="s">
+      <c r="Y16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Z16" s="7" t="s">
+      <c r="Z16" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA16" s="4" t="s">
@@ -2786,10 +2789,10 @@
       <c r="X26" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Y26" s="7" t="s">
+      <c r="Y26" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="Z26" s="7" t="s">
+      <c r="Z26" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA26" s="4" t="s">
@@ -2851,10 +2854,10 @@
       <c r="X27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Y27" s="7" t="s">
+      <c r="Y27" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="Z27" s="7" t="s">
+      <c r="Z27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="AA27" s="4" t="s">
@@ -2935,10 +2938,9 @@
       <c r="X28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Y28" s="7" t="s">
+      <c r="Y28" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="Z28" s="7"/>
       <c r="AA28" s="4" t="s">
         <v>25</v>
       </c>
@@ -3023,10 +3025,9 @@
       <c r="X29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Y29" s="7" t="s">
+      <c r="Y29" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="Z29" s="7"/>
       <c r="AA29" s="4" t="s">
         <v>25</v>
       </c>
@@ -3108,10 +3109,10 @@
       <c r="X30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y30" s="7" t="s">
+      <c r="Y30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Z30" s="7" t="s">
+      <c r="Z30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="AA30" s="4" t="s">
@@ -3192,10 +3193,10 @@
       <c r="X31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y31" s="7" t="s">
+      <c r="Y31" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="Z31" s="7" t="s">
+      <c r="Z31" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA31" s="4" t="s">
@@ -3276,10 +3277,10 @@
       <c r="X32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y32" s="7" t="s">
+      <c r="Y32" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="Z32" s="7" t="s">
+      <c r="Z32" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA32" s="4" t="s">
@@ -3356,10 +3357,10 @@
       <c r="X33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y33" s="7" t="s">
+      <c r="Y33" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="Z33" s="7" t="s">
+      <c r="Z33" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA33" s="4" t="s">
@@ -3433,10 +3434,10 @@
       <c r="X34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y34" s="7" t="s">
+      <c r="Y34" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="Z34" s="7" t="s">
+      <c r="Z34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="AA34" s="4" t="s">
@@ -3510,10 +3511,10 @@
       <c r="X35" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y35" s="7" t="s">
+      <c r="Y35" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="Z35" s="7" t="s">
+      <c r="Z35" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA35" s="4" t="s">
@@ -3587,10 +3588,10 @@
       <c r="X36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y36" s="7" t="s">
+      <c r="Y36" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="Z36" s="7" t="s">
+      <c r="Z36" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA36" s="4" t="s">
@@ -3673,10 +3674,10 @@
       <c r="X37" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y37" s="7" t="s">
+      <c r="Y37" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="Z37" s="7" t="s">
+      <c r="Z37" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA37" s="4" t="s">
@@ -3759,10 +3760,10 @@
       <c r="X38" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y38" s="7" t="s">
+      <c r="Y38" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="Z38" s="7" t="s">
+      <c r="Z38" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA38" s="4" t="s">
@@ -3845,10 +3846,10 @@
       <c r="X39" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y39" s="7" t="s">
+      <c r="Y39" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="Z39" s="7" t="s">
+      <c r="Z39" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AA39" s="4" t="s">

</xml_diff>

<commit_message>
Added to data all median, se, range, iqr cols (need to carefully document all extraction)
</commit_message>
<xml_diff>
--- a/data/studies_data.xlsx
+++ b/data/studies_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Steele Research Ltd\Stronger by Science\pcos_ree_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A7C9AF-AE33-4372-9019-1C9340A58305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFE1137-7908-4819-989D-4975CCC35B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="174">
   <si>
     <t>study</t>
   </si>
@@ -276,9 +276,6 @@
   </si>
   <si>
     <t>Canada</t>
-  </si>
-  <si>
-    <t>white</t>
   </si>
   <si>
     <t>Australia</t>
@@ -515,6 +512,54 @@
   </si>
   <si>
     <t>Hyperinsulinemic euglycemic clamp technique, M-value (mg/kg/min, median) = 11.9 (IQR = 9.4-14.5)</t>
+  </si>
+  <si>
+    <t>OGTT (75g oral glucose load), Fasting insulin (uIU/ml) = 6.32 (SE = 0.3), Fasting glucose:insulin ratio = 14.84 (SE = 1.19), HOMA = 103.38 (9.85), QUICKI = 0.38 (SE = 0)</t>
+  </si>
+  <si>
+    <t>OGTT (75g oral glucose load), Fasting insulin (uIU/ml) = 20.86 (SE = 1.13), Fasting glucose:insulin ratio = 4.24 (SE = 0.18), HOMA = 25.27 (1.41), QUICKI = 0.31 (SE = 0)</t>
+  </si>
+  <si>
+    <t>Assumed that the authors have reported SD instead of SEM for their REE in this group given the values</t>
+  </si>
+  <si>
+    <t>Assumed that the authors have reported SD instead of SEM for their age in this group given the values</t>
+  </si>
+  <si>
+    <t>median_age</t>
+  </si>
+  <si>
+    <t>se_age</t>
+  </si>
+  <si>
+    <t>median_body_mass</t>
+  </si>
+  <si>
+    <t>se_body_mass</t>
+  </si>
+  <si>
+    <t>median_fat_mass</t>
+  </si>
+  <si>
+    <t>se_fat_mass</t>
+  </si>
+  <si>
+    <t>median_fat_free_mass</t>
+  </si>
+  <si>
+    <t>se_fat_free_mass</t>
+  </si>
+  <si>
+    <t>median_height</t>
+  </si>
+  <si>
+    <t>se_height</t>
+  </si>
+  <si>
+    <t>median_bmi</t>
+  </si>
+  <si>
+    <t>se_bmi</t>
   </si>
 </sst>
 </file>
@@ -589,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -607,6 +652,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -943,12 +994,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE7CBA6-16D3-4F56-AAFF-D7A43475C68F}">
-  <dimension ref="A1:AY39"/>
+  <dimension ref="A1:CC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="V34" sqref="V34"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,9 +1009,9 @@
     <col min="8" max="16384" width="27.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -984,136 +1035,226 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="AX1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:51" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1139,64 +1280,64 @@
         <v>22</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J2" s="4">
         <v>23.3</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>5.2</v>
       </c>
-      <c r="N2" s="4">
+      <c r="X2" s="4">
         <v>27.1</v>
       </c>
-      <c r="O2" s="4">
+      <c r="Z2" s="4">
         <v>14.4</v>
       </c>
-      <c r="P2" s="4">
+      <c r="AE2" s="4">
         <v>49</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="AG2" s="4">
         <v>7.7</v>
       </c>
-      <c r="T2" s="4">
+      <c r="AS2" s="4">
         <v>28.3</v>
       </c>
-      <c r="U2" s="4">
+      <c r="AU2" s="4">
         <v>7.4</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" s="4" t="s">
+      <c r="BC2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="BD2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="BF2" s="4">
         <v>266</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="BH2" s="4">
         <v>1509</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="BJ2" s="4">
         <v>201</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="BV2" s="4">
         <v>31.8</v>
       </c>
-      <c r="AT2" s="4">
+      <c r="BX2" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:51" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1222,64 +1363,64 @@
         <v>23</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" s="4">
         <v>25.2</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <v>3.6</v>
       </c>
-      <c r="N3" s="4">
+      <c r="X3" s="4">
         <v>13.6</v>
       </c>
-      <c r="O3" s="4">
+      <c r="Z3" s="4">
         <v>5.4</v>
       </c>
-      <c r="P3" s="4">
+      <c r="AE3" s="4">
         <v>42.8</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="AG3" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="T3" s="4">
+      <c r="AS3" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="U3" s="4">
+      <c r="AU3" s="4">
         <v>2</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="BB3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z3" s="4" t="s">
+      <c r="BC3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="BF3" s="4">
         <v>51</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" s="4">
+      <c r="BH3" s="4">
         <v>1554</v>
       </c>
-      <c r="AF3" s="4">
+      <c r="BJ3" s="4">
         <v>277</v>
       </c>
-      <c r="AR3" s="4">
+      <c r="BV3" s="4">
         <v>35.4</v>
       </c>
-      <c r="AT3" s="4">
+      <c r="BX3" s="4">
         <v>3.9</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1305,52 +1446,52 @@
         <v>22</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" s="4">
         <v>23.5</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>6.3</v>
       </c>
-      <c r="T4" s="4">
+      <c r="AS4" s="4">
         <v>29.4</v>
       </c>
-      <c r="U4" s="4">
+      <c r="AU4" s="4">
         <v>6.4</v>
       </c>
-      <c r="V4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="X4" s="4" t="s">
+      <c r="AZ4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BA4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="BB4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA4" s="4" t="s">
+      <c r="BC4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="BD4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="BF4" s="4">
         <v>84</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="BG4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="BH4" s="4">
         <v>1463</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="BJ4" s="4">
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -1376,52 +1517,52 @@
         <v>23</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" s="4">
         <v>26.2</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>6.5</v>
       </c>
-      <c r="T5" s="4">
+      <c r="AS5" s="4">
         <v>27.2</v>
       </c>
-      <c r="U5" s="4">
+      <c r="AU5" s="4">
         <v>5.8</v>
       </c>
-      <c r="V5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="X5" s="4" t="s">
+      <c r="AZ5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z5" s="4" t="s">
+      <c r="BC5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="BE5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="BF5" s="4">
         <v>54</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="BH5" s="4">
         <v>1468</v>
       </c>
-      <c r="AF5" s="4">
+      <c r="BJ5" s="4">
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -1447,52 +1588,52 @@
         <v>22</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="4">
         <v>22.7</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>6.2</v>
       </c>
-      <c r="T6" s="4">
+      <c r="AS6" s="4">
         <v>28.9</v>
       </c>
-      <c r="U6" s="4">
+      <c r="AU6" s="4">
         <v>5.6</v>
       </c>
-      <c r="V6" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="X6" s="4" t="s">
+      <c r="AZ6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="BB6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA6" s="4" t="s">
+      <c r="BC6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="BF6" s="4">
         <v>61</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="BG6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD6" s="4">
+      <c r="BH6" s="4">
         <v>1469</v>
       </c>
-      <c r="AF6" s="4">
+      <c r="BJ6" s="4">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -1518,52 +1659,52 @@
         <v>23</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="4">
         <v>25</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>5.6</v>
       </c>
-      <c r="T7" s="4">
+      <c r="AS7" s="4">
         <v>27.1</v>
       </c>
-      <c r="U7" s="4">
+      <c r="AU7" s="4">
         <v>5.7</v>
       </c>
-      <c r="V7" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="X7" s="4" t="s">
+      <c r="AZ7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Y7" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z7" s="4" t="s">
+      <c r="BC7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA7" s="4" t="s">
+      <c r="BE7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="BF7" s="4">
         <v>44</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="BG7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD7" s="4">
+      <c r="BH7" s="4">
         <v>1453</v>
       </c>
-      <c r="AF7" s="4">
+      <c r="BJ7" s="4">
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -1589,49 +1730,49 @@
         <v>22</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J8" s="4">
         <v>30.8</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>5.4</v>
       </c>
-      <c r="L8" s="4">
+      <c r="Q8" s="4">
         <v>85.3</v>
       </c>
-      <c r="M8" s="4">
+      <c r="S8" s="4">
         <v>13.1</v>
       </c>
-      <c r="T8" s="4">
+      <c r="AS8" s="4">
         <v>32.6</v>
       </c>
-      <c r="U8" s="4">
+      <c r="AU8" s="4">
         <v>3.7</v>
       </c>
-      <c r="W8" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="X8" s="4" t="s">
+      <c r="BA8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AA8" s="4" t="s">
+      <c r="BE8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB8" s="4">
+      <c r="BF8" s="4">
         <v>30</v>
       </c>
-      <c r="AC8" s="4" t="s">
+      <c r="BG8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD8" s="4">
+      <c r="BH8" s="4">
         <v>1677</v>
       </c>
-      <c r="AF8" s="4">
+      <c r="BJ8" s="4">
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:51" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -1657,70 +1798,70 @@
         <v>22</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J9" s="4">
         <v>28.6</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>5</v>
       </c>
-      <c r="L9" s="4">
+      <c r="Q9" s="4">
         <v>104.1</v>
       </c>
-      <c r="M9" s="4">
+      <c r="S9" s="4">
         <v>19.3</v>
       </c>
-      <c r="N9" s="4">
+      <c r="X9" s="4">
         <v>51.6</v>
       </c>
-      <c r="O9" s="4">
+      <c r="Z9" s="4">
         <v>15.4</v>
       </c>
-      <c r="P9" s="4">
+      <c r="AE9" s="4">
         <v>52.5</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="AG9" s="4">
         <v>7.5</v>
       </c>
-      <c r="T9" s="4">
+      <c r="AS9" s="4">
         <v>39.9</v>
       </c>
-      <c r="U9" s="4">
+      <c r="AU9" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="AZ9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BA9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BB9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC9" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="W9" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="X9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA9" s="4" t="s">
+      <c r="BD9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="BF9" s="4">
         <v>28</v>
       </c>
-      <c r="AC9" s="4" t="s">
+      <c r="BG9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD9" s="4">
+      <c r="BH9" s="4">
         <v>1689</v>
       </c>
-      <c r="AF9" s="4">
+      <c r="BJ9" s="4">
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -1746,71 +1887,71 @@
         <v>22</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" s="4">
         <v>26</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>5.2</v>
       </c>
-      <c r="N10" s="4">
+      <c r="X10" s="4">
         <v>41.2</v>
       </c>
-      <c r="O10" s="4">
+      <c r="Z10" s="4">
         <v>12.5</v>
       </c>
-      <c r="P10" s="4">
+      <c r="AE10" s="4">
         <v>56.3</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="AG10" s="4">
         <v>5</v>
       </c>
-      <c r="T10" s="4">
+      <c r="AS10" s="4">
         <v>34.1</v>
       </c>
-      <c r="U10" s="4">
+      <c r="AU10" s="4">
         <v>3.6</v>
       </c>
-      <c r="V10" s="4" t="s">
+      <c r="AZ10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="W10" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="X10" s="4" t="s">
+      <c r="BB10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y10" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="AA10" s="4" t="s">
+      <c r="BC10" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="BF10" s="4">
         <v>6</v>
       </c>
-      <c r="AC10" s="4" t="s">
+      <c r="BG10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AE10" s="4">
+      <c r="BI10" s="4">
         <v>1411</v>
       </c>
-      <c r="AJ10" s="4">
+      <c r="BN10" s="4">
         <v>245</v>
       </c>
-      <c r="AL10" s="4">
+      <c r="BP10" s="4">
         <v>1411</v>
       </c>
-      <c r="AQ10" s="4">
+      <c r="BU10" s="4">
         <f>1613-1368</f>
         <v>245</v>
       </c>
-      <c r="AY10" s="4" t="s">
-        <v>121</v>
+      <c r="CC10" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1836,71 +1977,71 @@
         <v>22</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" s="4">
         <v>27</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="4">
         <v>3.7</v>
       </c>
-      <c r="N11" s="4">
+      <c r="X11" s="4">
         <v>23.3</v>
       </c>
-      <c r="O11" s="4">
+      <c r="Z11" s="4">
         <v>6.9</v>
       </c>
-      <c r="P11" s="4">
+      <c r="AE11" s="4">
         <v>47.4</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="AG11" s="4">
         <v>5.6</v>
       </c>
-      <c r="T11" s="4">
+      <c r="AS11" s="4">
         <v>26.4</v>
       </c>
-      <c r="U11" s="4">
+      <c r="AU11" s="4">
         <v>3</v>
       </c>
-      <c r="V11" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="X11" s="4" t="s">
+      <c r="AZ11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="BB11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y11" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA11" s="4" t="s">
+      <c r="BC11" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="BE11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB11" s="4">
+      <c r="BF11" s="4">
         <v>8</v>
       </c>
-      <c r="AC11" s="4" t="s">
+      <c r="BG11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AE11" s="4">
+      <c r="BI11" s="4">
         <v>1274</v>
       </c>
-      <c r="AJ11" s="4">
+      <c r="BN11" s="4">
         <v>181</v>
       </c>
-      <c r="AL11" s="4">
+      <c r="BP11" s="4">
         <v>1274</v>
       </c>
-      <c r="AQ11" s="4">
+      <c r="BU11" s="4">
         <f>1355-1174</f>
         <v>181</v>
       </c>
-      <c r="AY11" s="4" t="s">
-        <v>121</v>
+      <c r="CC11" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>5</v>
       </c>
@@ -1926,71 +2067,71 @@
         <v>23</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J12" s="4">
         <v>23</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="4">
         <v>0.7</v>
       </c>
-      <c r="N12" s="4">
+      <c r="X12" s="4">
         <v>17.100000000000001</v>
       </c>
-      <c r="O12" s="4">
+      <c r="Z12" s="4">
         <v>7.6</v>
       </c>
-      <c r="P12" s="4">
+      <c r="AE12" s="4">
         <v>45.9</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="AG12" s="4">
         <v>6.7</v>
       </c>
-      <c r="T12" s="4">
+      <c r="AS12" s="4">
         <v>22.5</v>
       </c>
-      <c r="U12" s="4">
+      <c r="AU12" s="4">
         <v>3.6</v>
       </c>
-      <c r="V12" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="X12" s="4" t="s">
+      <c r="AZ12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y12" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA12" s="4" t="s">
+      <c r="BC12" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="BE12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB12" s="4">
+      <c r="BF12" s="4">
         <v>10</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="BG12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AE12" s="4">
+      <c r="BI12" s="4">
         <v>1239</v>
       </c>
-      <c r="AJ12" s="4">
+      <c r="BN12" s="4">
         <v>259</v>
       </c>
-      <c r="AL12" s="4">
+      <c r="BP12" s="4">
         <v>1239</v>
       </c>
-      <c r="AQ12" s="4">
+      <c r="BU12" s="4">
         <f>1454-1195</f>
         <v>259</v>
       </c>
-      <c r="AY12" s="4" t="s">
-        <v>121</v>
+      <c r="CC12" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:81" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -2016,52 +2157,52 @@
         <v>22</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J13" s="4">
         <v>30.2</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L13" s="4">
+      <c r="Q13" s="4">
         <v>79.599999999999994</v>
       </c>
-      <c r="M13" s="4">
+      <c r="S13" s="4">
         <v>20.3</v>
       </c>
-      <c r="R13" s="4">
+      <c r="AL13" s="4">
         <v>167.3</v>
       </c>
-      <c r="S13" s="4">
+      <c r="AN13" s="4">
         <v>6.8</v>
       </c>
-      <c r="T13" s="4">
+      <c r="AS13" s="4">
         <v>28.5</v>
       </c>
-      <c r="U13" s="4">
+      <c r="AU13" s="4">
         <v>7.2</v>
       </c>
-      <c r="X13" s="4" t="s">
+      <c r="BB13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AA13" s="4" t="s">
+      <c r="BE13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB13" s="4">
+      <c r="BF13" s="4">
         <v>72</v>
       </c>
-      <c r="AC13" s="4" t="s">
+      <c r="BG13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD13" s="4">
+      <c r="BH13" s="4">
         <v>1411</v>
       </c>
-      <c r="AF13" s="4">
+      <c r="BJ13" s="4">
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:51" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:81" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>6</v>
       </c>
@@ -2087,52 +2228,52 @@
         <v>23</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J14" s="4">
         <v>27.8</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>3.6</v>
       </c>
-      <c r="L14" s="4">
+      <c r="Q14" s="4">
         <v>70.900000000000006</v>
       </c>
-      <c r="M14" s="4">
+      <c r="S14" s="4">
         <v>17.100000000000001</v>
       </c>
-      <c r="R14" s="4">
+      <c r="AL14" s="4">
         <v>169</v>
       </c>
-      <c r="S14" s="4">
+      <c r="AN14" s="4">
         <v>6.5</v>
       </c>
-      <c r="T14" s="4">
+      <c r="AS14" s="4">
         <v>24.6</v>
       </c>
-      <c r="U14" s="4">
+      <c r="AU14" s="4">
         <v>5</v>
       </c>
-      <c r="X14" s="4" t="s">
+      <c r="BB14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="4" t="s">
+      <c r="BE14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB14" s="4">
+      <c r="BF14" s="4">
         <v>30</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="BG14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD14" s="4">
+      <c r="BH14" s="4">
         <v>1325</v>
       </c>
-      <c r="AF14" s="4">
+      <c r="BJ14" s="4">
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:51" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:81" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>7</v>
       </c>
@@ -2158,75 +2299,75 @@
         <v>22</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" s="4">
         <v>29.6</v>
       </c>
-      <c r="K15" s="4">
+      <c r="L15" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L15" s="4">
+      <c r="Q15" s="4">
         <v>105.4</v>
       </c>
-      <c r="M15" s="4">
+      <c r="S15" s="4">
         <v>14.5</v>
       </c>
-      <c r="N15" s="4">
+      <c r="X15" s="4">
         <v>52.4</v>
       </c>
-      <c r="O15" s="4">
+      <c r="Z15" s="4">
         <v>14.8</v>
       </c>
-      <c r="P15" s="4">
+      <c r="AE15" s="4">
         <v>52.3</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="AG15" s="4">
         <v>10.7</v>
       </c>
-      <c r="T15" s="4">
+      <c r="AS15" s="4">
         <v>38.5</v>
       </c>
-      <c r="U15" s="4">
+      <c r="AU15" s="4">
         <v>4.2</v>
       </c>
-      <c r="V15" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="W15" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="X15" s="4" t="s">
+      <c r="AZ15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BA15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA15" s="4" t="s">
+      <c r="BC15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB15" s="4">
+      <c r="BF15" s="4">
         <v>10</v>
       </c>
-      <c r="AC15" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK15" s="4">
+      <c r="BG15" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BO15" s="4">
         <f>0.21*2*24</f>
         <v>10.08</v>
       </c>
-      <c r="AM15" s="4">
+      <c r="BQ15" s="4">
         <f>0.02*2*24</f>
         <v>0.96</v>
       </c>
-      <c r="AY15" s="4" t="s">
-        <v>84</v>
+      <c r="CC15" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:51" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:81" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>7</v>
       </c>
@@ -2252,225 +2393,255 @@
         <v>22</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J16" s="4">
         <v>29.6</v>
       </c>
-      <c r="K16" s="4">
+      <c r="L16" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L16" s="4">
+      <c r="Q16" s="4">
         <v>97.3</v>
       </c>
-      <c r="M16" s="4">
+      <c r="S16" s="4">
         <v>13.9</v>
       </c>
-      <c r="N16" s="4">
+      <c r="X16" s="4">
         <v>45.7</v>
       </c>
-      <c r="O16" s="4">
+      <c r="Z16" s="4">
         <v>12.5</v>
       </c>
-      <c r="P16" s="4">
+      <c r="AE16" s="4">
         <v>50.5</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="AG16" s="4">
         <v>11.4</v>
       </c>
-      <c r="T16" s="4">
+      <c r="AS16" s="4">
         <v>35.5</v>
       </c>
-      <c r="U16" s="4">
+      <c r="AU16" s="4">
         <v>4.5</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="W16" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="X16" s="4" t="s">
+      <c r="AZ16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BA16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y16" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA16" s="4" t="s">
+      <c r="BC16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB16" s="4">
+      <c r="BF16" s="4">
         <v>10</v>
       </c>
-      <c r="AC16" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK16" s="4">
+      <c r="BG16" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BO16" s="4">
         <f>0.21*2*24</f>
         <v>10.08</v>
       </c>
-      <c r="AM16" s="4">
+      <c r="BQ16" s="4">
         <f>0.02*2*24</f>
         <v>0.96</v>
       </c>
-      <c r="AY16" s="4" t="s">
-        <v>84</v>
+      <c r="CC16" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:51" s="2" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17" spans="1:81" s="7" customFormat="1" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>8</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="7">
         <v>9</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="7">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="8">
         <v>2009</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="I17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="7">
         <v>23.56</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="7">
         <v>4.6119843885251823</v>
       </c>
-      <c r="T17" s="2">
+      <c r="AS17" s="7">
         <v>24.79</v>
       </c>
-      <c r="U17" s="2">
+      <c r="AU17" s="7">
         <v>5.1545707871752038</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="BB17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="BC17" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="BF17" s="7">
         <v>46</v>
       </c>
+      <c r="BH17" s="7">
+        <v>1553.87</v>
+      </c>
+      <c r="BJ17" s="7">
+        <v>805.9</v>
+      </c>
+      <c r="CC17" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="18" spans="1:51" s="2" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:81" s="7" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>8</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="7">
         <v>9</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="7">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="8">
         <v>2009</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="I18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="7">
         <v>23.97</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="7">
         <v>5.15</v>
       </c>
-      <c r="T18" s="2">
+      <c r="AS18" s="7">
         <v>30.45</v>
       </c>
-      <c r="U18" s="2">
+      <c r="AU18" s="7">
         <v>7.55</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="BB18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AA18" s="2" t="s">
+      <c r="BC18" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="BE18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="BF18" s="7">
         <v>25</v>
       </c>
+      <c r="BH18" s="7">
+        <v>1174.56</v>
+      </c>
+      <c r="BJ18" s="7">
+        <v>454.38</v>
+      </c>
+      <c r="CC18" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="19" spans="1:51" s="2" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:81" s="7" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>8</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="7">
         <v>9</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="7">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="8">
         <v>2009</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="I19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="7">
         <v>25.17</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="7">
         <v>5.4039985196148974</v>
       </c>
-      <c r="T19" s="2">
+      <c r="AS19" s="7">
         <v>23.7</v>
       </c>
-      <c r="U19" s="2">
+      <c r="AU19" s="7">
         <v>7.0667672948810187</v>
       </c>
-      <c r="X19" s="2" t="s">
+      <c r="BB19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AA19" s="2" t="s">
+      <c r="BE19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="BF19" s="7">
         <v>48</v>
       </c>
+      <c r="BH19" s="7">
+        <v>1841.05</v>
+      </c>
+      <c r="BK19" s="7">
+        <v>44</v>
+      </c>
     </row>
-    <row r="20" spans="1:51" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:81" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>8</v>
       </c>
@@ -2496,25 +2667,42 @@
         <v>22</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J20" s="2">
         <v>23.98</v>
       </c>
-      <c r="T20" s="2">
+      <c r="L20" s="2">
+        <v>5</v>
+      </c>
+      <c r="AL20" s="2">
+        <v>164</v>
+      </c>
+      <c r="AN20" s="2">
+        <f>1.4*SQRT(78)</f>
+        <v>12.364465212858986</v>
+      </c>
+      <c r="AS20" s="2">
         <v>26.7</v>
       </c>
-      <c r="X20" s="2" t="s">
+      <c r="AU20" s="2">
+        <f>1.6*SQRT(74)</f>
+        <v>13.763720427268204</v>
+      </c>
+      <c r="BB20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA20" s="2" t="s">
+      <c r="BE20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="BF20" s="2">
         <v>109</v>
       </c>
+      <c r="CC20" s="7" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="21" spans="1:51" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:81" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>8</v>
       </c>
@@ -2540,25 +2728,29 @@
         <v>23</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J21" s="2">
         <v>27</v>
       </c>
-      <c r="T21" s="2">
+      <c r="L21" s="2">
+        <f>1*SQRT(114)</f>
+        <v>10.677078252031311</v>
+      </c>
+      <c r="AS21" s="2">
         <v>19.100000000000001</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="BB21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA21" s="2" t="s">
+      <c r="BE21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="BF21" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:81" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>8</v>
       </c>
@@ -2584,25 +2776,25 @@
         <v>23</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J22" s="2">
         <v>34</v>
       </c>
-      <c r="T22" s="2">
+      <c r="AS22" s="2">
         <v>19.100000000000001</v>
       </c>
-      <c r="X22" s="2" t="s">
+      <c r="BB22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA22" s="2" t="s">
+      <c r="BE22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB22" s="2">
+      <c r="BF22" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:51" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:81" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>8</v>
       </c>
@@ -2628,31 +2820,31 @@
         <v>22</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J23" s="2">
         <v>24</v>
       </c>
-      <c r="L23" s="2">
+      <c r="Q23" s="2">
         <v>72.5</v>
       </c>
-      <c r="N23" s="2">
+      <c r="X23" s="2">
         <v>164</v>
       </c>
-      <c r="T23" s="2">
+      <c r="AS23" s="2">
         <v>27.41</v>
       </c>
-      <c r="X23" s="2" t="s">
+      <c r="BB23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA23" s="2" t="s">
+      <c r="BE23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB23" s="2">
+      <c r="BF23" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:51" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:81" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>8</v>
       </c>
@@ -2678,28 +2870,28 @@
         <v>22</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J24" s="2">
         <v>22.82</v>
       </c>
-      <c r="T24" s="2">
+      <c r="AS24" s="2">
         <v>25.7</v>
       </c>
-      <c r="V24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="X24" s="2" t="s">
+      <c r="AZ24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA24" s="2" t="s">
+      <c r="BE24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB24" s="2">
+      <c r="BF24" s="2">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:51" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:81" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>8</v>
       </c>
@@ -2725,28 +2917,28 @@
         <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J25" s="2">
         <v>22.91</v>
       </c>
-      <c r="T25" s="2">
+      <c r="AS25" s="2">
         <v>21.190999999999999</v>
       </c>
-      <c r="V25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="X25" s="2" t="s">
+      <c r="AZ25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA25" s="2" t="s">
+      <c r="BE25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB25" s="2">
+      <c r="BF25" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>9</v>
       </c>
@@ -2772,46 +2964,46 @@
         <v>22</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J26" s="4">
         <v>25.9</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>5.3</v>
       </c>
-      <c r="T26" s="4">
+      <c r="AS26" s="4">
         <v>26.97</v>
       </c>
-      <c r="U26" s="4">
+      <c r="AU26" s="4">
         <v>5.12</v>
       </c>
-      <c r="X26" s="4" t="s">
+      <c r="BB26" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Y26" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA26" s="4" t="s">
+      <c r="BC26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB26" s="4">
+      <c r="BF26" s="4">
         <v>31</v>
       </c>
-      <c r="AC26" s="4" t="s">
+      <c r="BG26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD26" s="4">
+      <c r="BH26" s="4">
         <v>1166.8699999999999</v>
       </c>
-      <c r="AF26" s="4">
+      <c r="BJ26" s="4">
         <v>370.98</v>
       </c>
     </row>
-    <row r="27" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>9</v>
       </c>
@@ -2837,46 +3029,46 @@
         <v>23</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J27" s="4">
         <v>27.1</v>
       </c>
-      <c r="K27" s="4">
+      <c r="L27" s="4">
         <v>4.8</v>
       </c>
-      <c r="T27" s="4">
+      <c r="AS27" s="4">
         <v>26.03</v>
       </c>
-      <c r="U27" s="4">
+      <c r="AU27" s="4">
         <v>5.66</v>
       </c>
-      <c r="X27" s="4" t="s">
+      <c r="BB27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Y27" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z27" s="4" t="s">
+      <c r="BC27" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA27" s="4" t="s">
+      <c r="BE27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB27" s="4">
+      <c r="BF27" s="4">
         <v>29</v>
       </c>
-      <c r="AC27" s="4" t="s">
+      <c r="BG27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD27" s="4">
+      <c r="BH27" s="4">
         <v>1045.52</v>
       </c>
-      <c r="AF27" s="4">
+      <c r="BJ27" s="4">
         <v>295.86</v>
       </c>
     </row>
-    <row r="28" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>10</v>
       </c>
@@ -2902,68 +3094,68 @@
         <v>22</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J28" s="4">
         <v>27</v>
       </c>
-      <c r="K28" s="4">
+      <c r="L28" s="4">
         <f>(42-20)/4</f>
         <v>5.5</v>
       </c>
-      <c r="L28" s="4">
+      <c r="Q28" s="4">
         <v>70.25</v>
       </c>
-      <c r="M28" s="4">
+      <c r="S28" s="4">
         <f>AVERAGE((71.1-53.5)/4,(118.2-74.3)/4)</f>
         <v>7.6875</v>
       </c>
-      <c r="P28" s="4">
+      <c r="AE28" s="4">
         <v>50.150000000000006</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="AG28" s="4">
         <f>AVERAGE((54-44.1)/4,(60.1-46)/4)</f>
         <v>3</v>
       </c>
-      <c r="T28" s="4">
+      <c r="AS28" s="4">
         <v>27.049999999999997</v>
       </c>
-      <c r="U28" s="4">
+      <c r="AU28" s="4">
         <f>AVERAGE((24.4-19.2)/4,(48.7-27)/4)</f>
         <v>3.3625000000000003</v>
       </c>
-      <c r="V28" s="4" t="s">
+      <c r="AZ28" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC28" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="X28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y28" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA28" s="4" t="s">
+      <c r="BE28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB28" s="4">
+      <c r="BF28" s="4">
         <v>14</v>
       </c>
-      <c r="AC28" s="4" t="s">
+      <c r="BG28" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AE28" s="4">
+      <c r="BI28" s="4">
         <v>6796</v>
       </c>
-      <c r="AH28" s="4">
+      <c r="BL28" s="4">
         <v>5489</v>
       </c>
-      <c r="AI28" s="4">
+      <c r="BM28" s="4">
         <v>7774</v>
       </c>
-      <c r="AY28" s="4" t="s">
-        <v>131</v>
+      <c r="CC28" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:51" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:81" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>10</v>
       </c>
@@ -2989,68 +3181,68 @@
         <v>23</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J29" s="4">
         <v>29</v>
       </c>
-      <c r="K29" s="4">
+      <c r="L29" s="4">
         <f>(40-23)/4</f>
         <v>4.25</v>
       </c>
-      <c r="L29" s="4">
+      <c r="Q29" s="4">
         <v>71.25</v>
       </c>
-      <c r="M29" s="4">
+      <c r="S29" s="4">
         <f>AVERAGE((73.9-48.5)/4,(114.5-77.2)/4)</f>
         <v>7.8375000000000004</v>
       </c>
-      <c r="P29" s="4">
+      <c r="AE29" s="4">
         <v>50.6</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="AG29" s="4">
         <f>AVERAGE((56.9-36.8)/4,(63.3-48.7)/4)</f>
         <v>4.3374999999999995</v>
       </c>
-      <c r="T29" s="4">
+      <c r="AS29" s="4">
         <v>27.85</v>
       </c>
-      <c r="U29" s="4">
+      <c r="AU29" s="4">
         <f>AVERAGE((24-18.6)/4,(41.3-26.7)/4)</f>
         <v>2.4999999999999996</v>
       </c>
-      <c r="V29" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="X29" s="4" t="s">
+      <c r="AZ29" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Y29" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA29" s="4" t="s">
+      <c r="BC29" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BE29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB29" s="4">
+      <c r="BF29" s="4">
         <v>14</v>
       </c>
-      <c r="AC29" s="4" t="s">
+      <c r="BG29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AE29" s="4">
+      <c r="BI29" s="4">
         <v>6833</v>
       </c>
-      <c r="AH29" s="4">
+      <c r="BL29" s="4">
         <v>4893</v>
       </c>
-      <c r="AI29" s="4">
+      <c r="BM29" s="4">
         <v>8492</v>
       </c>
-      <c r="AY29" s="4" t="s">
-        <v>131</v>
+      <c r="CC29" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:51" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:81" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>11</v>
       </c>
@@ -3076,65 +3268,65 @@
         <v>23</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J30" s="4">
         <v>28</v>
       </c>
-      <c r="K30" s="4">
+      <c r="L30" s="4">
         <f>1*SQRT(11)</f>
         <v>3.3166247903553998</v>
       </c>
-      <c r="L30" s="4">
+      <c r="Q30" s="4">
         <v>62.5</v>
       </c>
-      <c r="M30" s="4">
+      <c r="S30" s="4">
         <f>1.5*SQRT(11)</f>
         <v>4.9749371855330997</v>
       </c>
-      <c r="P30" s="4">
+      <c r="AE30" s="4">
         <v>48.8</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="AG30" s="4">
         <f>1.4*SQRT(11)</f>
         <v>4.643274706497559</v>
       </c>
-      <c r="R30" s="4">
+      <c r="AL30" s="4">
         <v>171</v>
       </c>
-      <c r="S30" s="4">
+      <c r="AN30" s="4">
         <f>1*SQRT(11)</f>
         <v>3.3166247903553998</v>
       </c>
-      <c r="X30" s="4" t="s">
+      <c r="BB30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y30" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z30" s="4" t="s">
+      <c r="BC30" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="BD30" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA30" s="4" t="s">
+      <c r="BE30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB30" s="4">
+      <c r="BF30" s="4">
         <v>11</v>
       </c>
-      <c r="AC30" s="4" t="s">
+      <c r="BG30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD30" s="4">
+      <c r="BH30" s="4">
         <v>1481.7599999999998</v>
       </c>
-      <c r="AG30" s="4">
+      <c r="BK30" s="4">
         <v>33.119999999999997</v>
       </c>
-      <c r="AY30" s="4" t="s">
-        <v>85</v>
+      <c r="CC30" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:51" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:81" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>11</v>
       </c>
@@ -3160,65 +3352,65 @@
         <v>23</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J31" s="4">
         <v>29</v>
       </c>
-      <c r="K31" s="4">
+      <c r="L31" s="4">
         <f>2*SQRT(9)</f>
         <v>6</v>
       </c>
-      <c r="L31" s="4">
+      <c r="Q31" s="4">
         <v>86.9</v>
       </c>
-      <c r="M31" s="4">
+      <c r="S31" s="4">
         <f>5.8*SQRT(9)</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="P31" s="4">
+      <c r="AE31" s="4">
         <v>50.4</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="AG31" s="4">
         <f>1.4*SQRT(9)</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="R31" s="4">
+      <c r="AL31" s="4">
         <v>164</v>
       </c>
-      <c r="S31" s="4">
+      <c r="AN31" s="4">
         <f>3*SQRT(9)</f>
         <v>9</v>
       </c>
-      <c r="X31" s="4" t="s">
+      <c r="BB31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y31" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA31" s="4" t="s">
+      <c r="BC31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="BD31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="4">
+      <c r="BF31" s="4">
         <v>9</v>
       </c>
-      <c r="AC31" s="4" t="s">
+      <c r="BG31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD31" s="4">
+      <c r="BH31" s="4">
         <v>1558.0800000000002</v>
       </c>
-      <c r="AG31" s="4">
+      <c r="BK31" s="4">
         <v>61.919999999999995</v>
       </c>
-      <c r="AY31" s="4" t="s">
-        <v>85</v>
+      <c r="CC31" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:51" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:81" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>11</v>
       </c>
@@ -3244,65 +3436,65 @@
         <v>22</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J32" s="4">
         <v>25</v>
       </c>
-      <c r="K32" s="4">
+      <c r="L32" s="4">
         <f>2*SQRT(10)</f>
         <v>6.324555320336759</v>
       </c>
-      <c r="L32" s="4">
+      <c r="Q32" s="4">
         <v>84.1</v>
       </c>
-      <c r="M32" s="4">
+      <c r="S32" s="4">
         <f>2.7*SQRT(10)</f>
         <v>8.538149682454625</v>
       </c>
-      <c r="P32" s="4">
+      <c r="AE32" s="4">
         <v>48.7</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="AG32" s="4">
         <f>1.3*SQRT(10)</f>
         <v>4.110960958218894</v>
       </c>
-      <c r="R32" s="4">
+      <c r="AL32" s="4">
         <v>163</v>
       </c>
-      <c r="S32" s="4">
+      <c r="AN32" s="4">
         <f>2*SQRT(10)</f>
         <v>6.324555320336759</v>
       </c>
-      <c r="X32" s="4" t="s">
+      <c r="BB32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Y32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA32" s="4" t="s">
+      <c r="BC32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BD32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="4">
+      <c r="BF32" s="4">
         <v>10</v>
       </c>
-      <c r="AC32" s="4" t="s">
+      <c r="BG32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD32" s="4">
+      <c r="BH32" s="4">
         <v>1507.6799999999998</v>
       </c>
-      <c r="AG32" s="4">
+      <c r="BK32" s="4">
         <v>53.279999999999994</v>
       </c>
-      <c r="AY32" s="4" t="s">
-        <v>85</v>
+      <c r="CC32" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:33" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:63" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>12</v>
       </c>
@@ -3328,58 +3520,58 @@
         <v>22</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J33" s="4">
         <v>32.299999999999997</v>
       </c>
-      <c r="K33" s="4">
+      <c r="L33" s="4">
         <f>1*SQRT(7)</f>
         <v>2.6457513110645907</v>
       </c>
-      <c r="L33" s="4">
+      <c r="Q33" s="4">
         <v>100.5</v>
       </c>
-      <c r="M33" s="4">
+      <c r="S33" s="4">
         <f>6.7*SQRT(7)</f>
         <v>17.726533784132759</v>
       </c>
-      <c r="T33" s="4">
+      <c r="AS33" s="4">
         <v>36.200000000000003</v>
       </c>
-      <c r="U33" s="4">
+      <c r="AU33" s="4">
         <f>2*SQRT(7)</f>
         <v>5.2915026221291814</v>
       </c>
-      <c r="W33" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="X33" s="4" t="s">
+      <c r="BA33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="BB33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y33" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA33" s="4" t="s">
+      <c r="BC33" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB33" s="4">
+      <c r="BF33" s="4">
         <v>7</v>
       </c>
-      <c r="AC33" s="4" t="s">
+      <c r="BG33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD33" s="4">
+      <c r="BH33" s="4">
         <v>1485</v>
       </c>
-      <c r="AG33" s="4">
+      <c r="BK33" s="4">
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:33" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:63" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>12</v>
       </c>
@@ -3405,58 +3597,58 @@
         <v>22</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J34" s="4">
         <v>32.299999999999997</v>
       </c>
-      <c r="K34" s="4">
+      <c r="L34" s="4">
         <f>1*SQRT(7)</f>
         <v>2.6457513110645907</v>
       </c>
-      <c r="L34" s="4">
+      <c r="Q34" s="4">
         <v>99.7</v>
       </c>
-      <c r="M34" s="4">
+      <c r="S34" s="4">
         <f>7.5*SQRT(7)</f>
         <v>19.843134832984429</v>
       </c>
-      <c r="T34" s="4">
+      <c r="AS34" s="4">
         <v>35.9</v>
       </c>
-      <c r="U34" s="4">
+      <c r="AU34" s="4">
         <f>2.2*SQRT(7)</f>
         <v>5.8206528843420999</v>
       </c>
-      <c r="W34" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="X34" s="4" t="s">
+      <c r="BA34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y34" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z34" s="4" t="s">
+      <c r="BC34" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="BD34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA34" s="4" t="s">
+      <c r="BE34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB34" s="4">
+      <c r="BF34" s="4">
         <v>7</v>
       </c>
-      <c r="AC34" s="4" t="s">
+      <c r="BG34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD34" s="4">
+      <c r="BH34" s="4">
         <v>1610</v>
       </c>
-      <c r="AG34" s="4">
+      <c r="BK34" s="4">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:33" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:63" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>12</v>
       </c>
@@ -3482,58 +3674,58 @@
         <v>22</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J35" s="4">
         <v>28.4</v>
       </c>
-      <c r="K35" s="4">
+      <c r="L35" s="4">
         <f>2.7*SQRT(5)</f>
         <v>6.0373835392494328</v>
       </c>
-      <c r="L35" s="4">
+      <c r="Q35" s="4">
         <v>94.8</v>
       </c>
-      <c r="M35" s="4">
+      <c r="S35" s="4">
         <f>6.2*SQRT(5)</f>
         <v>13.863621460498697</v>
       </c>
-      <c r="T35" s="4">
+      <c r="AS35" s="4">
         <v>37.1</v>
       </c>
-      <c r="U35" s="4">
+      <c r="AU35" s="4">
         <f>3.4*SQRT(5)</f>
         <v>7.6026311234992852</v>
       </c>
-      <c r="W35" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="X35" s="4" t="s">
+      <c r="BA35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="BB35" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y35" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA35" s="4" t="s">
+      <c r="BC35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="BD35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB35" s="4">
+      <c r="BF35" s="4">
         <v>5</v>
       </c>
-      <c r="AC35" s="4" t="s">
+      <c r="BG35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD35" s="4">
+      <c r="BH35" s="4">
         <v>1596</v>
       </c>
-      <c r="AG35" s="4">
+      <c r="BK35" s="4">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:33" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:63" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>12</v>
       </c>
@@ -3559,58 +3751,58 @@
         <v>22</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J36" s="4">
         <v>28.4</v>
       </c>
-      <c r="K36" s="4">
+      <c r="L36" s="4">
         <f>2.7*SQRT(5)</f>
         <v>6.0373835392494328</v>
       </c>
-      <c r="L36" s="4">
+      <c r="Q36" s="4">
         <v>91.7</v>
       </c>
-      <c r="M36" s="4">
+      <c r="S36" s="4">
         <f>4.9*SQRT(5)</f>
         <v>10.956733089748971</v>
       </c>
-      <c r="T36" s="4">
+      <c r="AS36" s="4">
         <v>35.9</v>
       </c>
-      <c r="U36" s="4">
+      <c r="AU36" s="4">
         <f>3*SQRT(5)</f>
         <v>6.7082039324993694</v>
       </c>
-      <c r="W36" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="X36" s="4" t="s">
+      <c r="BA36" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Y36" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA36" s="4" t="s">
+      <c r="BC36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB36" s="4">
+      <c r="BF36" s="4">
         <v>5</v>
       </c>
-      <c r="AC36" s="4" t="s">
+      <c r="BG36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AD36" s="4">
+      <c r="BH36" s="4">
         <v>1586</v>
       </c>
-      <c r="AG36" s="4">
+      <c r="BK36" s="4">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:33" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:63" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>13</v>
       </c>
@@ -3636,67 +3828,67 @@
         <v>22</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J37" s="4">
         <v>32.1</v>
       </c>
-      <c r="K37" s="4">
+      <c r="L37" s="4">
         <v>5.2</v>
       </c>
-      <c r="L37" s="4">
+      <c r="Q37" s="4">
         <v>96</v>
       </c>
-      <c r="M37" s="4">
+      <c r="S37" s="4">
         <f>3.3*SQRT(34)</f>
         <v>19.242141252989491</v>
       </c>
-      <c r="N37" s="4">
+      <c r="X37" s="4">
         <v>34.9</v>
       </c>
-      <c r="O37" s="4">
+      <c r="Z37" s="4">
         <f>1.5*SQRT(34)</f>
         <v>8.746427842267952</v>
       </c>
-      <c r="P37" s="4">
+      <c r="AE37" s="4">
         <v>61.5</v>
       </c>
-      <c r="Q37" s="4">
+      <c r="AG37" s="4">
         <f>2.1*SQRT(34)</f>
         <v>12.244998979175133</v>
       </c>
-      <c r="V37" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="W37" s="4" t="s">
+      <c r="AZ37" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BA37" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC37" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="X37" s="4" t="s">
+      <c r="BD37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BF37" s="4">
+        <v>34</v>
+      </c>
+      <c r="BG37" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y37" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="Z37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB37" s="4">
-        <v>34</v>
-      </c>
-      <c r="AC37" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD37" s="4">
+      <c r="BH37" s="4">
         <v>7.7</v>
       </c>
-      <c r="AG37" s="4">
+      <c r="BK37" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="38" spans="1:33" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:63" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>13</v>
       </c>
@@ -3722,67 +3914,67 @@
         <v>22</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J38" s="4">
         <v>32.1</v>
       </c>
-      <c r="K38" s="4">
+      <c r="L38" s="4">
         <v>5.2</v>
       </c>
-      <c r="L38" s="4">
+      <c r="Q38" s="4">
         <v>90.3</v>
       </c>
-      <c r="M38" s="4">
+      <c r="S38" s="4">
         <f>3.3*SQRT(34)</f>
         <v>19.242141252989491</v>
       </c>
-      <c r="N38" s="4">
+      <c r="X38" s="4">
         <v>30.8</v>
       </c>
-      <c r="O38" s="4">
+      <c r="Z38" s="4">
         <f>1.6*SQRT(34)</f>
         <v>9.3295230317524815</v>
       </c>
-      <c r="P38" s="4">
+      <c r="AE38" s="4">
         <v>59.8</v>
       </c>
-      <c r="Q38" s="4">
+      <c r="AG38" s="4">
         <f>1.9*SQRT(34)</f>
         <v>11.07880860020607</v>
       </c>
-      <c r="V38" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="W38" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="X38" s="4" t="s">
+      <c r="AZ38" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BA38" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB38" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC38" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BF38" s="4">
+        <v>34</v>
+      </c>
+      <c r="BG38" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y38" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB38" s="4">
-        <v>34</v>
-      </c>
-      <c r="AC38" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD38" s="4">
+      <c r="BH38" s="4">
         <v>7.1</v>
       </c>
-      <c r="AG38" s="4">
+      <c r="BK38" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:33" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:63" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>13</v>
       </c>
@@ -3808,63 +4000,63 @@
         <v>22</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J39" s="4">
         <v>32.1</v>
       </c>
-      <c r="K39" s="4">
+      <c r="L39" s="4">
         <v>5.2</v>
       </c>
-      <c r="L39" s="4">
+      <c r="Q39" s="4">
         <v>92.5</v>
       </c>
-      <c r="M39" s="4">
+      <c r="S39" s="4">
         <f>4.4*SQRT(23)</f>
         <v>21.101658702575964</v>
       </c>
-      <c r="N39" s="4">
+      <c r="X39" s="4">
         <v>32.4</v>
       </c>
-      <c r="O39" s="4">
+      <c r="Z39" s="4">
         <f>2.1*SQRT(23)</f>
         <v>10.071246198956711</v>
       </c>
-      <c r="P39" s="4">
+      <c r="AE39" s="4">
         <v>60.1</v>
       </c>
-      <c r="Q39" s="4">
+      <c r="AG39" s="4">
         <f>2.5*SQRT(23)</f>
         <v>11.989578808281799</v>
       </c>
-      <c r="V39" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="W39" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="X39" s="4" t="s">
+      <c r="AZ39" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BA39" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC39" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="BD39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BF39" s="4">
+        <v>23</v>
+      </c>
+      <c r="BG39" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y39" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA39" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB39" s="4">
-        <v>23</v>
-      </c>
-      <c r="AC39" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD39" s="4">
+      <c r="BH39" s="4">
         <v>7.4</v>
       </c>
-      <c r="AG39" s="4">
+      <c r="BK39" s="4">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove ® from device cells in data
</commit_message>
<xml_diff>
--- a/data/studies_data.xlsx
+++ b/data/studies_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Steele Research Ltd\Stronger by Science\pcos_ree_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B88653A-8BDD-48C9-B351-527CDCC178DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98AA010-D9AF-47F9-BD0D-D09FED7FA9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
   </bookViews>
@@ -598,9 +598,6 @@
     <t>Quark RMR instrument (Cosmed, Cernusco sul Naviglio, Italy) equipped with a ventilated hood</t>
   </si>
   <si>
-    <t>Fitmate® (Cosmed, Rome, Italy)</t>
-  </si>
-  <si>
     <t>Oral dose (1.0 g/kg bodyweight) of amixture that contained 1 part deuterium (2H 99.9% enriched) and 19 parts Oxygen-18 (18O10% enriched), followed by 100 mL of tap water used to rinse the dose container.</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>PCOS was diagnosed by elevation of one or more plasma and androgen levels in the presence of chronic oligomenorrhea or ammenorrhea.</t>
+  </si>
+  <si>
+    <t>Fitmate (Cosmed, Rome, Italy)</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -776,12 +776,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1120,10 +1114,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE7CBA6-16D3-4F56-AAFF-D7A43475C68F}">
   <dimension ref="A1:CK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+      <selection pane="bottomLeft" activeCell="BM4" sqref="BM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>89</v>
@@ -1186,7 +1180,7 @@
         <v>168</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>98</v>
@@ -1210,7 +1204,7 @@
         <v>171</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>99</v>
@@ -1234,7 +1228,7 @@
         <v>174</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>100</v>
@@ -1258,7 +1252,7 @@
         <v>177</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>101</v>
@@ -1282,7 +1276,7 @@
         <v>180</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>102</v>
@@ -1306,7 +1300,7 @@
         <v>183</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>51</v>
@@ -1428,7 +1422,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>90</v>
@@ -1603,7 +1597,7 @@
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>90</v>
@@ -1639,7 +1633,7 @@
         <v>25</v>
       </c>
       <c r="BM4" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="BN4" s="1">
         <v>84</v>
@@ -1713,7 +1707,7 @@
         <v>25</v>
       </c>
       <c r="BM5" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="BN5" s="1">
         <v>54</v>
@@ -1754,7 +1748,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>90</v>
@@ -1790,7 +1784,7 @@
         <v>25</v>
       </c>
       <c r="BM6" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="BN6" s="1">
         <v>61</v>
@@ -1864,7 +1858,7 @@
         <v>25</v>
       </c>
       <c r="BM7" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="BN7" s="1">
         <v>44</v>
@@ -1905,7 +1899,7 @@
         <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>90</v>
@@ -1938,7 +1932,7 @@
         <v>25</v>
       </c>
       <c r="BM8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BN8" s="1">
         <v>30</v>
@@ -1979,7 +1973,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>90</v>
@@ -2063,7 +2057,7 @@
         <v>60</v>
       </c>
       <c r="BM9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BN9" s="1">
         <v>28</v>
@@ -2110,7 +2104,7 @@
         <v>22</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>90</v>
@@ -2159,7 +2153,7 @@
         <v>25</v>
       </c>
       <c r="BM10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BN10" s="1">
         <v>6</v>
@@ -2207,7 +2201,7 @@
         <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>90</v>
@@ -2256,7 +2250,7 @@
         <v>25</v>
       </c>
       <c r="BM11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BN11" s="1">
         <v>8</v>
@@ -2350,7 +2344,7 @@
         <v>25</v>
       </c>
       <c r="BM12" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BN12" s="1">
         <v>10</v>
@@ -2398,7 +2392,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>90</v>
@@ -2434,7 +2428,7 @@
         <v>25</v>
       </c>
       <c r="BM13" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BN13" s="1">
         <v>72</v>
@@ -2508,7 +2502,7 @@
         <v>25</v>
       </c>
       <c r="BM14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BN14" s="1">
         <v>30</v>
@@ -2549,7 +2543,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>90</v>
@@ -2603,7 +2597,7 @@
         <v>25</v>
       </c>
       <c r="BM15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BN15" s="1">
         <v>10</v>
@@ -2620,7 +2614,7 @@
         <v>0.96</v>
       </c>
       <c r="CK15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:89" ht="135" x14ac:dyDescent="0.25">
@@ -2649,7 +2643,7 @@
         <v>22</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>91</v>
@@ -2703,7 +2697,7 @@
         <v>25</v>
       </c>
       <c r="BM16" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BN16" s="1">
         <v>10</v>
@@ -2720,7 +2714,7 @@
         <v>0.96</v>
       </c>
       <c r="CK16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:89" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2749,7 +2743,7 @@
         <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>90</v>
@@ -2776,7 +2770,7 @@
         <v>73</v>
       </c>
       <c r="BJ17" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BK17" s="1" t="s">
         <v>2</v>
@@ -2785,7 +2779,7 @@
         <v>25</v>
       </c>
       <c r="BM17" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN17" s="1">
         <v>46</v>
@@ -2800,7 +2794,7 @@
         <v>805.9</v>
       </c>
       <c r="CK17" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:89" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2829,7 +2823,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>90</v>
@@ -2856,7 +2850,7 @@
         <v>73</v>
       </c>
       <c r="BJ18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BK18" s="1" t="s">
         <v>38</v>
@@ -2865,7 +2859,7 @@
         <v>25</v>
       </c>
       <c r="BM18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN18" s="1">
         <v>25</v>
@@ -2880,7 +2874,7 @@
         <v>454.38</v>
       </c>
       <c r="CK18" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -2930,7 +2924,7 @@
         <v>25</v>
       </c>
       <c r="BM19" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN19" s="1">
         <v>48</v>
@@ -2945,7 +2939,7 @@
         <v>44</v>
       </c>
       <c r="CK19" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:89" ht="135" x14ac:dyDescent="0.25">
@@ -2974,7 +2968,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>90</v>
@@ -3025,7 +3019,7 @@
         <v>73</v>
       </c>
       <c r="BJ20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BK20" s="1" t="s">
         <v>2</v>
@@ -3034,7 +3028,7 @@
         <v>25</v>
       </c>
       <c r="BM20" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN20" s="1">
         <v>73</v>
@@ -3049,7 +3043,7 @@
         <v>167.9</v>
       </c>
       <c r="CK20" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -3105,7 +3099,7 @@
         <v>25</v>
       </c>
       <c r="BM21" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN21" s="1">
         <v>114</v>
@@ -3114,7 +3108,7 @@
         <v>58</v>
       </c>
       <c r="CK21" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -3170,7 +3164,7 @@
         <v>25</v>
       </c>
       <c r="BM22" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN22" s="1">
         <v>47</v>
@@ -3179,7 +3173,7 @@
         <v>58</v>
       </c>
       <c r="CK22" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:89" ht="135" x14ac:dyDescent="0.25">
@@ -3208,7 +3202,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>90</v>
@@ -3253,7 +3247,7 @@
         <v>73</v>
       </c>
       <c r="BJ23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BK23" s="1" t="s">
         <v>38</v>
@@ -3262,7 +3256,7 @@
         <v>25</v>
       </c>
       <c r="BM23" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN23" s="1">
         <v>63</v>
@@ -3277,7 +3271,7 @@
         <v>83.2</v>
       </c>
       <c r="CK23" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:89" ht="105" x14ac:dyDescent="0.25">
@@ -3306,7 +3300,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>90</v>
@@ -3342,7 +3336,7 @@
         <v>73</v>
       </c>
       <c r="BJ24" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BK24" s="1" t="s">
         <v>2</v>
@@ -3351,7 +3345,7 @@
         <v>25</v>
       </c>
       <c r="BM24" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN24" s="1">
         <v>156</v>
@@ -3366,7 +3360,7 @@
         <v>672.9</v>
       </c>
       <c r="CK24" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -3419,7 +3413,7 @@
         <v>25</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BN25" s="1">
         <v>56</v>
@@ -3428,1218 +3422,1218 @@
         <v>58</v>
       </c>
       <c r="CK25" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:89" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="1:89" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>9</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="1">
         <v>13</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="1">
         <v>24</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="2">
         <v>2008</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J26" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="1">
         <v>25.9</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26" s="1">
         <v>5.3</v>
       </c>
-      <c r="AY26" s="4">
+      <c r="AY26" s="1">
         <v>26.97</v>
       </c>
-      <c r="BA26" s="4">
+      <c r="BA26" s="1">
         <v>5.12</v>
       </c>
-      <c r="BI26" s="4" t="s">
+      <c r="BI26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BJ26" s="4" t="s">
+      <c r="BJ26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BK26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL26" s="4" t="s">
+      <c r="BK26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="BM26" s="4" t="s">
+      <c r="BM26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="BN26" s="1">
+        <v>31</v>
+      </c>
+      <c r="BO26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP26" s="1">
+        <v>1166.8699999999999</v>
+      </c>
+      <c r="BR26" s="1">
+        <v>370.98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:89" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2008</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K27" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="AY27" s="1">
+        <v>26.03</v>
+      </c>
+      <c r="BA27" s="1">
+        <v>5.66</v>
+      </c>
+      <c r="BI27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BJ27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="BK27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM27" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="BN27" s="1">
+        <v>29</v>
+      </c>
+      <c r="BO27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP27" s="1">
+        <v>1045.52</v>
+      </c>
+      <c r="BR27" s="1">
+        <v>295.86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:89" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1992</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L28" s="1">
+        <v>27</v>
+      </c>
+      <c r="O28" s="1">
+        <v>20</v>
+      </c>
+      <c r="P28" s="1">
+        <v>42</v>
+      </c>
+      <c r="T28" s="1">
+        <v>70.25</v>
+      </c>
+      <c r="W28" s="1">
+        <v>53.5</v>
+      </c>
+      <c r="X28" s="1">
+        <v>118.2</v>
+      </c>
+      <c r="AJ28" s="1">
+        <v>50.150000000000006</v>
+      </c>
+      <c r="AM28" s="1">
+        <v>44.1</v>
+      </c>
+      <c r="AN28" s="1">
+        <v>60.1</v>
+      </c>
+      <c r="AY28" s="1">
+        <v>27.049999999999997</v>
+      </c>
+      <c r="BC28" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="BD28" s="1">
+        <v>48.7</v>
+      </c>
+      <c r="BG28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="BI28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BL28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM28" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BN28" s="1">
+        <v>14</v>
+      </c>
+      <c r="BO28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ28" s="1">
+        <v>6796</v>
+      </c>
+      <c r="BT28" s="1">
+        <v>5489</v>
+      </c>
+      <c r="BU28" s="1">
+        <v>7774</v>
+      </c>
+      <c r="CK28" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="BN26" s="4">
+    </row>
+    <row r="29" spans="1:89" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1992</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29" s="1">
+        <v>29</v>
+      </c>
+      <c r="O29" s="1">
+        <v>23</v>
+      </c>
+      <c r="P29" s="1">
+        <v>40</v>
+      </c>
+      <c r="T29" s="1">
+        <v>71.25</v>
+      </c>
+      <c r="W29" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="X29" s="1">
+        <v>114.5</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>50.6</v>
+      </c>
+      <c r="AM29" s="1">
+        <v>36</v>
+      </c>
+      <c r="AN29" s="1">
+        <v>63.3</v>
+      </c>
+      <c r="AY29" s="1">
+        <v>27.85</v>
+      </c>
+      <c r="BC29" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="BD29" s="1">
+        <v>41.3</v>
+      </c>
+      <c r="BG29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="BI29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BL29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM29" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BN29" s="1">
+        <v>14</v>
+      </c>
+      <c r="BO29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ29" s="1">
+        <v>6833</v>
+      </c>
+      <c r="BT29" s="1">
+        <v>4893</v>
+      </c>
+      <c r="BU29" s="1">
+        <v>8492</v>
+      </c>
+      <c r="CK29" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:89" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1">
+        <v>28</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1990</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" s="1">
+        <v>28</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="V30" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AI30" s="1">
+        <v>48.8</v>
+      </c>
+      <c r="AL30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="1">
+        <v>171</v>
+      </c>
+      <c r="AT30" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BK30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN30" s="1">
+        <v>11</v>
+      </c>
+      <c r="BO30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP30" s="1">
+        <v>1481.7599999999998</v>
+      </c>
+      <c r="BS30" s="1">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="CK30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:89" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1">
+        <v>29</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1990</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" s="1">
+        <v>29</v>
+      </c>
+      <c r="N31" s="1">
+        <v>2</v>
+      </c>
+      <c r="S31" s="1">
+        <v>86.9</v>
+      </c>
+      <c r="V31" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="AI31" s="1">
+        <v>50.4</v>
+      </c>
+      <c r="AL31" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AQ31" s="1">
+        <v>164</v>
+      </c>
+      <c r="AT31" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BK31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN31" s="1">
+        <v>9</v>
+      </c>
+      <c r="BO31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP31" s="1">
+        <v>1558.0800000000002</v>
+      </c>
+      <c r="BS31" s="1">
+        <v>61.919999999999995</v>
+      </c>
+      <c r="CK31" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:89" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1">
+        <v>30</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1990</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32" s="1">
+        <v>25</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2</v>
+      </c>
+      <c r="S32" s="1">
+        <v>84.1</v>
+      </c>
+      <c r="V32" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AI32" s="1">
+        <v>48.7</v>
+      </c>
+      <c r="AL32" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="AQ32" s="1">
+        <v>163</v>
+      </c>
+      <c r="AT32" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BK32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN32" s="1">
+        <v>10</v>
+      </c>
+      <c r="BO32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP32" s="1">
+        <v>1507.6799999999998</v>
+      </c>
+      <c r="BS32" s="1">
+        <v>53.279999999999994</v>
+      </c>
+      <c r="CK32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:89" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1">
         <v>31</v>
       </c>
-      <c r="BO26" s="4" t="s">
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K33" s="1">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="N33" s="1">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1">
+        <v>100.5</v>
+      </c>
+      <c r="V33" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="AY33" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="BB33" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BK33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM33" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BN33" s="1">
+        <v>7</v>
+      </c>
+      <c r="BO33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BP26" s="4">
-        <v>1166.8699999999999</v>
-      </c>
-      <c r="BR26" s="4">
-        <v>370.98</v>
+      <c r="BP33" s="1">
+        <v>1485</v>
+      </c>
+      <c r="BQ33" s="1">
+        <v>1469</v>
+      </c>
+      <c r="BS33" s="1">
+        <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:89" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>9</v>
-      </c>
-      <c r="B27" s="4">
+    <row r="34" spans="1:89" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1">
+        <v>16</v>
+      </c>
+      <c r="C34" s="1">
+        <v>31</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K34" s="1">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="N34" s="1">
+        <v>1</v>
+      </c>
+      <c r="S34" s="1">
+        <v>99.7</v>
+      </c>
+      <c r="V34" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="AY34" s="1">
+        <v>35.9</v>
+      </c>
+      <c r="BB34" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BH34" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM34" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BN34" s="1">
+        <v>7</v>
+      </c>
+      <c r="BO34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP34" s="1">
+        <v>1610</v>
+      </c>
+      <c r="BQ34" s="1">
+        <v>1452</v>
+      </c>
+      <c r="BS34" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:89" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1">
+        <v>16</v>
+      </c>
+      <c r="C35" s="1">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="S35" s="1">
+        <v>94.8</v>
+      </c>
+      <c r="V35" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="AY35" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="BB35" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="BH35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BK35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM35" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BN35" s="1">
+        <v>5</v>
+      </c>
+      <c r="BO35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP35" s="1">
+        <v>1596</v>
+      </c>
+      <c r="BQ35" s="1">
+        <v>1653</v>
+      </c>
+      <c r="BS35" s="1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:89" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1">
+        <v>16</v>
+      </c>
+      <c r="C36" s="1">
+        <v>32</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="N36" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="S36" s="1">
+        <v>91.7</v>
+      </c>
+      <c r="V36" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AY36" s="1">
+        <v>35.9</v>
+      </c>
+      <c r="BB36" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BI36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BK36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM36" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BN36" s="1">
+        <v>5</v>
+      </c>
+      <c r="BO36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BP36" s="1">
+        <v>1586</v>
+      </c>
+      <c r="BQ36" s="1">
+        <v>1530</v>
+      </c>
+      <c r="BS36" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:89" ht="180" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>13</v>
       </c>
-      <c r="C27" s="4">
-        <v>25</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="B37" s="1">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1">
         <v>33</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="5">
-        <v>2008</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="4" t="s">
+      <c r="D37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K27" s="4">
-        <v>27.1</v>
-      </c>
-      <c r="M27" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="AY27" s="4">
-        <v>26.03</v>
-      </c>
-      <c r="BA27" s="4">
-        <v>5.66</v>
-      </c>
-      <c r="BI27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="BJ27" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BK27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BL27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM27" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="BN27" s="4">
-        <v>29</v>
-      </c>
-      <c r="BO27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP27" s="4">
-        <v>1045.52</v>
-      </c>
-      <c r="BR27" s="4">
-        <v>295.86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:89" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>10</v>
-      </c>
-      <c r="B28" s="4">
-        <v>14</v>
-      </c>
-      <c r="C28" s="4">
-        <v>26</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="5">
-        <v>1992</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L28" s="4">
-        <v>27</v>
-      </c>
-      <c r="O28" s="4">
-        <v>20</v>
-      </c>
-      <c r="P28" s="4">
-        <v>42</v>
-      </c>
-      <c r="T28" s="4">
-        <v>70.25</v>
-      </c>
-      <c r="W28" s="4">
-        <v>53.5</v>
-      </c>
-      <c r="X28" s="4">
-        <v>118.2</v>
-      </c>
-      <c r="AJ28" s="4">
-        <v>50.150000000000006</v>
-      </c>
-      <c r="AM28" s="4">
-        <v>44.1</v>
-      </c>
-      <c r="AN28" s="4">
-        <v>60.1</v>
-      </c>
-      <c r="AY28" s="4">
-        <v>27.049999999999997</v>
-      </c>
-      <c r="BC28" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="BD28" s="4">
-        <v>48.7</v>
-      </c>
-      <c r="BG28" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="BI28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="BJ28" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="BL28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM28" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="BN28" s="4">
-        <v>14</v>
-      </c>
-      <c r="BO28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="BQ28" s="4">
-        <v>6796</v>
-      </c>
-      <c r="BT28" s="4">
-        <v>5489</v>
-      </c>
-      <c r="BU28" s="4">
-        <v>7774</v>
-      </c>
-      <c r="CK28" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="29" spans="1:89" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4">
-        <v>14</v>
-      </c>
-      <c r="C29" s="4">
-        <v>27</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1992</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L29" s="4">
-        <v>29</v>
-      </c>
-      <c r="O29" s="4">
-        <v>23</v>
-      </c>
-      <c r="P29" s="4">
-        <v>40</v>
-      </c>
-      <c r="T29" s="4">
-        <v>71.25</v>
-      </c>
-      <c r="W29" s="4">
-        <v>49.5</v>
-      </c>
-      <c r="X29" s="4">
-        <v>114.5</v>
-      </c>
-      <c r="AJ29" s="4">
-        <v>50.6</v>
-      </c>
-      <c r="AM29" s="4">
-        <v>36</v>
-      </c>
-      <c r="AN29" s="4">
-        <v>63.3</v>
-      </c>
-      <c r="AY29" s="4">
-        <v>27.85</v>
-      </c>
-      <c r="BC29" s="4">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="BD29" s="4">
-        <v>41.3</v>
-      </c>
-      <c r="BG29" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="BI29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="BJ29" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="BL29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM29" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="BN29" s="4">
-        <v>14</v>
-      </c>
-      <c r="BO29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="BQ29" s="4">
-        <v>6833</v>
-      </c>
-      <c r="BT29" s="4">
-        <v>4893</v>
-      </c>
-      <c r="BU29" s="4">
-        <v>8492</v>
-      </c>
-      <c r="CK29" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="30" spans="1:89" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>11</v>
-      </c>
-      <c r="B30" s="4">
-        <v>15</v>
-      </c>
-      <c r="C30" s="4">
-        <v>28</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1990</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K30" s="4">
-        <v>28</v>
-      </c>
-      <c r="N30" s="4">
-        <v>1</v>
-      </c>
-      <c r="S30" s="4">
-        <v>62.5</v>
-      </c>
-      <c r="V30" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="AI30" s="4">
-        <v>48.8</v>
-      </c>
-      <c r="AL30" s="4">
-        <v>1</v>
-      </c>
-      <c r="AQ30" s="4">
-        <v>171</v>
-      </c>
-      <c r="AT30" s="4">
-        <v>1</v>
-      </c>
-      <c r="BI30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ30" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BK30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BL30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM30" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="BN30" s="4">
-        <v>11</v>
-      </c>
-      <c r="BO30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP30" s="4">
-        <v>1481.7599999999998</v>
-      </c>
-      <c r="BS30" s="4">
-        <v>33.119999999999997</v>
-      </c>
-      <c r="CK30" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:89" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>11</v>
-      </c>
-      <c r="B31" s="4">
-        <v>15</v>
-      </c>
-      <c r="C31" s="4">
-        <v>29</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1990</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K31" s="4">
-        <v>29</v>
-      </c>
-      <c r="N31" s="4">
-        <v>2</v>
-      </c>
-      <c r="S31" s="4">
-        <v>86.9</v>
-      </c>
-      <c r="V31" s="4">
-        <v>5.8</v>
-      </c>
-      <c r="AI31" s="4">
-        <v>50.4</v>
-      </c>
-      <c r="AL31" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="AQ31" s="4">
-        <v>164</v>
-      </c>
-      <c r="AT31" s="4">
-        <v>3</v>
-      </c>
-      <c r="BI31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ31" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BK31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL31" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM31" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="BN31" s="4">
-        <v>9</v>
-      </c>
-      <c r="BO31" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP31" s="4">
-        <v>1558.0800000000002</v>
-      </c>
-      <c r="BS31" s="4">
-        <v>61.919999999999995</v>
-      </c>
-      <c r="CK31" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:89" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>11</v>
-      </c>
-      <c r="B32" s="4">
-        <v>15</v>
-      </c>
-      <c r="C32" s="4">
-        <v>30</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="5">
-        <v>1990</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K32" s="4">
-        <v>25</v>
-      </c>
-      <c r="N32" s="4">
-        <v>2</v>
-      </c>
-      <c r="S32" s="4">
-        <v>84.1</v>
-      </c>
-      <c r="V32" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="AI32" s="4">
-        <v>48.7</v>
-      </c>
-      <c r="AL32" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="AQ32" s="4">
-        <v>163</v>
-      </c>
-      <c r="AT32" s="4">
-        <v>2</v>
-      </c>
-      <c r="BI32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ32" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BK32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM32" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="BN32" s="4">
-        <v>10</v>
-      </c>
-      <c r="BO32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP32" s="4">
-        <v>1507.6799999999998</v>
-      </c>
-      <c r="BS32" s="4">
-        <v>53.279999999999994</v>
-      </c>
-      <c r="CK32" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:89" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>12</v>
-      </c>
-      <c r="B33" s="4">
-        <v>16</v>
-      </c>
-      <c r="C33" s="4">
-        <v>31</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="4">
-        <v>2006</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K33" s="4">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="N33" s="4">
-        <v>1</v>
-      </c>
-      <c r="S33" s="4">
-        <v>100.5</v>
-      </c>
-      <c r="V33" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="AY33" s="4">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="BB33" s="4">
-        <v>2</v>
-      </c>
-      <c r="BH33" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="BI33" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ33" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="BK33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM33" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="BN33" s="4">
-        <v>7</v>
-      </c>
-      <c r="BO33" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP33" s="4">
-        <v>1485</v>
-      </c>
-      <c r="BQ33" s="4">
-        <v>1469</v>
-      </c>
-      <c r="BS33" s="4">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="1:89" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>12</v>
-      </c>
-      <c r="B34" s="4">
-        <v>16</v>
-      </c>
-      <c r="C34" s="4">
-        <v>31</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" s="4">
-        <v>2006</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K34" s="4">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="N34" s="4">
-        <v>1</v>
-      </c>
-      <c r="S34" s="4">
-        <v>99.7</v>
-      </c>
-      <c r="V34" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="AY34" s="4">
-        <v>35.9</v>
-      </c>
-      <c r="BB34" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="BH34" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="BI34" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ34" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="BK34" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BL34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM34" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="BN34" s="4">
-        <v>7</v>
-      </c>
-      <c r="BO34" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP34" s="4">
-        <v>1610</v>
-      </c>
-      <c r="BQ34" s="4">
-        <v>1452</v>
-      </c>
-      <c r="BS34" s="4">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:89" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>12</v>
-      </c>
-      <c r="B35" s="4">
-        <v>16</v>
-      </c>
-      <c r="C35" s="4">
-        <v>32</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="4">
-        <v>2006</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K35" s="4">
-        <v>28.4</v>
-      </c>
-      <c r="N35" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="S35" s="4">
-        <v>94.8</v>
-      </c>
-      <c r="V35" s="4">
-        <v>6.2</v>
-      </c>
-      <c r="AY35" s="4">
-        <v>37.1</v>
-      </c>
-      <c r="BB35" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="BH35" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="BI35" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ35" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="BK35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL35" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM35" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="BN35" s="4">
-        <v>5</v>
-      </c>
-      <c r="BO35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP35" s="4">
-        <v>1596</v>
-      </c>
-      <c r="BQ35" s="4">
-        <v>1653</v>
-      </c>
-      <c r="BS35" s="4">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:89" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>12</v>
-      </c>
-      <c r="B36" s="4">
-        <v>16</v>
-      </c>
-      <c r="C36" s="4">
-        <v>32</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="4">
-        <v>2006</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K36" s="4">
-        <v>28.4</v>
-      </c>
-      <c r="N36" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="S36" s="4">
-        <v>91.7</v>
-      </c>
-      <c r="V36" s="4">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="AY36" s="4">
-        <v>35.9</v>
-      </c>
-      <c r="BB36" s="4">
-        <v>3</v>
-      </c>
-      <c r="BH36" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="BI36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ36" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="BK36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BM36" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="BN36" s="4">
-        <v>5</v>
-      </c>
-      <c r="BO36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP36" s="4">
-        <v>1586</v>
-      </c>
-      <c r="BQ36" s="4">
-        <v>1530</v>
-      </c>
-      <c r="BS36" s="4">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:89" s="4" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>13</v>
-      </c>
-      <c r="B37" s="4">
-        <v>17</v>
-      </c>
-      <c r="C37" s="4">
-        <v>33</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="4">
-        <v>2006</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K37" s="4">
+      <c r="K37" s="1">
         <f>(33.2*16+32.1*18)/(16+18)</f>
         <v>32.617647058823529</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="1">
         <f>(4.8*16+5.5*18)/(16+18)</f>
         <v>5.1705882352941179</v>
       </c>
-      <c r="S37" s="4">
+      <c r="S37" s="1">
         <v>96</v>
       </c>
-      <c r="V37" s="4">
+      <c r="V37" s="1">
         <v>3.3</v>
       </c>
-      <c r="AA37" s="4">
+      <c r="AA37" s="1">
         <v>34.9</v>
       </c>
-      <c r="AD37" s="4">
+      <c r="AD37" s="1">
         <v>1.5</v>
       </c>
-      <c r="AI37" s="4">
+      <c r="AI37" s="1">
         <v>61.5</v>
       </c>
-      <c r="AL37" s="4">
+      <c r="AL37" s="1">
         <v>2.1</v>
       </c>
-      <c r="AY37" s="4">
+      <c r="AY37" s="1">
         <v>34.9</v>
       </c>
-      <c r="BA37" s="4">
+      <c r="BA37" s="1">
         <f>(7*16+6.6*18)/(16+18)</f>
         <v>6.7882352941176478</v>
       </c>
-      <c r="BG37" s="4" t="s">
+      <c r="BG37" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BH37" s="4" t="s">
+      <c r="BH37" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BI37" s="4" t="s">
+      <c r="BI37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BJ37" s="4" t="s">
+      <c r="BJ37" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BK37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL37" s="4" t="s">
+      <c r="BK37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="BM37" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="BN37" s="4">
+      <c r="BM37" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN37" s="1">
         <v>34</v>
       </c>
-      <c r="BO37" s="4" t="s">
+      <c r="BO37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BP37" s="4">
+      <c r="BP37" s="1">
         <v>7.7</v>
       </c>
-      <c r="BS37" s="4">
+      <c r="BS37" s="1">
         <v>0.3</v>
       </c>
-      <c r="CK37" s="4" t="s">
-        <v>212</v>
+      <c r="CK37" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:89" s="4" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+    <row r="38" spans="1:89" ht="225" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>13</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="1">
         <v>17</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="1">
         <v>33</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="D38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="1">
         <v>2006</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J38" s="4" t="s">
+      <c r="I38" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="1">
         <f t="shared" ref="K38:K39" si="0">(33.2*16+32.1*18)/(16+18)</f>
         <v>32.617647058823529</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="1">
         <f t="shared" ref="M38:M39" si="1">(4.8*16+5.5*18)/(16+18)</f>
         <v>5.1705882352941179</v>
       </c>
-      <c r="S38" s="4">
+      <c r="S38" s="1">
         <v>90.3</v>
       </c>
-      <c r="V38" s="4">
+      <c r="V38" s="1">
         <v>3.3</v>
       </c>
-      <c r="AA38" s="4">
+      <c r="AA38" s="1">
         <v>30.8</v>
       </c>
-      <c r="AD38" s="4">
+      <c r="AD38" s="1">
         <v>1.6</v>
       </c>
-      <c r="AI38" s="4">
+      <c r="AI38" s="1">
         <v>59.8</v>
       </c>
-      <c r="AL38" s="4">
+      <c r="AL38" s="1">
         <v>1.9</v>
       </c>
-      <c r="BG38" s="4" t="s">
+      <c r="BG38" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BH38" s="4" t="s">
+      <c r="BH38" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BI38" s="4" t="s">
+      <c r="BI38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BJ38" s="4" t="s">
+      <c r="BJ38" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BK38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL38" s="4" t="s">
+      <c r="BK38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="BM38" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="BN38" s="4">
+      <c r="BM38" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN38" s="1">
         <v>34</v>
       </c>
-      <c r="BO38" s="4" t="s">
+      <c r="BO38" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BP38" s="4">
+      <c r="BP38" s="1">
         <v>7.1</v>
       </c>
-      <c r="BS38" s="4">
+      <c r="BS38" s="1">
         <v>0.3</v>
       </c>
-      <c r="CK38" s="4" t="s">
-        <v>213</v>
+      <c r="CK38" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:89" s="4" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+    <row r="39" spans="1:89" ht="225" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>13</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="1">
         <v>17</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="1">
         <v>33</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="1">
         <v>2006</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J39" s="4" t="s">
+      <c r="I39" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="1">
         <f t="shared" si="0"/>
         <v>32.617647058823529</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="1">
         <f t="shared" si="1"/>
         <v>5.1705882352941179</v>
       </c>
-      <c r="S39" s="4">
+      <c r="S39" s="1">
         <v>92.5</v>
       </c>
-      <c r="V39" s="4">
+      <c r="V39" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AA39" s="4">
+      <c r="AA39" s="1">
         <v>32.4</v>
       </c>
-      <c r="AD39" s="4">
+      <c r="AD39" s="1">
         <v>2.1</v>
       </c>
-      <c r="AI39" s="4">
+      <c r="AI39" s="1">
         <v>60.1</v>
       </c>
-      <c r="AL39" s="4">
+      <c r="AL39" s="1">
         <v>2.5</v>
       </c>
-      <c r="BG39" s="4" t="s">
+      <c r="BG39" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BH39" s="4" t="s">
+      <c r="BH39" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BI39" s="4" t="s">
+      <c r="BI39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BJ39" s="4" t="s">
+      <c r="BJ39" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="BK39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL39" s="4" t="s">
+      <c r="BK39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="BM39" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="BN39" s="4">
+      <c r="BM39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN39" s="1">
         <v>23</v>
       </c>
-      <c r="BO39" s="4" t="s">
+      <c r="BO39" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BP39" s="4">
+      <c r="BP39" s="1">
         <v>7.4</v>
       </c>
-      <c r="BS39" s="4">
+      <c r="BS39" s="1">
         <v>0.3</v>
       </c>
-      <c r="CK39" s="4" t="s">
-        <v>213</v>
+      <c r="CK39" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove ™ from data too
</commit_message>
<xml_diff>
--- a/data/studies_data.xlsx
+++ b/data/studies_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox\Steele Research Ltd\Stronger by Science\pcos_ree_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98AA010-D9AF-47F9-BD0D-D09FED7FA9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B783BF06-A7CC-4259-AD9A-AE70DB8985EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{10DD01AD-3A16-4FAB-AD7D-B9DBF71733AB}"/>
   </bookViews>
@@ -607,9 +607,6 @@
     <t>Korr ReeVue indirect calorimetry (KorrMedical Technologies, Inc., Salt Lake City, UT 84120, USA)</t>
   </si>
   <si>
-    <t>Deltatrack™ II Metabolic Monitor ventilated hood system (Datex, Helsinki, Finland).</t>
-  </si>
-  <si>
     <t>ParvoMedics TrueOne 2400 Canopy System (ParvoMedics, Sandy, Utah, USA).</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>Fitmate (Cosmed, Rome, Italy)</t>
+  </si>
+  <si>
+    <t>Deltatrack II Metabolic Monitor ventilated hood system (Datex, Helsinki, Finland).</t>
   </si>
 </sst>
 </file>
@@ -1115,9 +1115,9 @@
   <dimension ref="A1:CK39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="BM4" sqref="BM4"/>
+      <selection pane="bottomLeft" activeCell="BM14" sqref="BM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>89</v>
@@ -1180,7 +1180,7 @@
         <v>168</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>98</v>
@@ -1204,7 +1204,7 @@
         <v>171</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>99</v>
@@ -1228,7 +1228,7 @@
         <v>174</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>100</v>
@@ -1252,7 +1252,7 @@
         <v>177</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>101</v>
@@ -1276,7 +1276,7 @@
         <v>180</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>102</v>
@@ -1300,7 +1300,7 @@
         <v>183</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>51</v>
@@ -1422,7 +1422,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>90</v>
@@ -1597,7 +1597,7 @@
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>90</v>
@@ -1633,7 +1633,7 @@
         <v>25</v>
       </c>
       <c r="BM4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BN4" s="1">
         <v>84</v>
@@ -1707,7 +1707,7 @@
         <v>25</v>
       </c>
       <c r="BM5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BN5" s="1">
         <v>54</v>
@@ -1748,7 +1748,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>90</v>
@@ -1784,7 +1784,7 @@
         <v>25</v>
       </c>
       <c r="BM6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BN6" s="1">
         <v>61</v>
@@ -1858,7 +1858,7 @@
         <v>25</v>
       </c>
       <c r="BM7" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BN7" s="1">
         <v>44</v>
@@ -1899,7 +1899,7 @@
         <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>90</v>
@@ -1973,7 +1973,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>90</v>
@@ -2104,7 +2104,7 @@
         <v>22</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>90</v>
@@ -2201,7 +2201,7 @@
         <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>90</v>
@@ -2392,7 +2392,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>90</v>
@@ -2428,7 +2428,7 @@
         <v>25</v>
       </c>
       <c r="BM13" s="1" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="BN13" s="1">
         <v>72</v>
@@ -2502,7 +2502,7 @@
         <v>25</v>
       </c>
       <c r="BM14" s="1" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="BN14" s="1">
         <v>30</v>
@@ -2543,7 +2543,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>90</v>
@@ -2597,7 +2597,7 @@
         <v>25</v>
       </c>
       <c r="BM15" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BN15" s="1">
         <v>10</v>
@@ -2614,7 +2614,7 @@
         <v>0.96</v>
       </c>
       <c r="CK15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:89" ht="135" x14ac:dyDescent="0.25">
@@ -2643,7 +2643,7 @@
         <v>22</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>91</v>
@@ -2697,7 +2697,7 @@
         <v>25</v>
       </c>
       <c r="BM16" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BN16" s="1">
         <v>10</v>
@@ -2714,7 +2714,7 @@
         <v>0.96</v>
       </c>
       <c r="CK16" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:89" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>90</v>
@@ -2770,7 +2770,7 @@
         <v>73</v>
       </c>
       <c r="BJ17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BK17" s="1" t="s">
         <v>2</v>
@@ -2779,7 +2779,7 @@
         <v>25</v>
       </c>
       <c r="BM17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN17" s="1">
         <v>46</v>
@@ -2794,7 +2794,7 @@
         <v>805.9</v>
       </c>
       <c r="CK17" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:89" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2823,7 +2823,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>90</v>
@@ -2850,7 +2850,7 @@
         <v>73</v>
       </c>
       <c r="BJ18" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="BK18" s="1" t="s">
         <v>38</v>
@@ -2859,7 +2859,7 @@
         <v>25</v>
       </c>
       <c r="BM18" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN18" s="1">
         <v>25</v>
@@ -2874,7 +2874,7 @@
         <v>454.38</v>
       </c>
       <c r="CK18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -2924,7 +2924,7 @@
         <v>25</v>
       </c>
       <c r="BM19" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN19" s="1">
         <v>48</v>
@@ -2939,7 +2939,7 @@
         <v>44</v>
       </c>
       <c r="CK19" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:89" ht="135" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>90</v>
@@ -3019,7 +3019,7 @@
         <v>73</v>
       </c>
       <c r="BJ20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BK20" s="1" t="s">
         <v>2</v>
@@ -3028,7 +3028,7 @@
         <v>25</v>
       </c>
       <c r="BM20" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN20" s="1">
         <v>73</v>
@@ -3043,7 +3043,7 @@
         <v>167.9</v>
       </c>
       <c r="CK20" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>25</v>
       </c>
       <c r="BM21" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN21" s="1">
         <v>114</v>
@@ -3108,7 +3108,7 @@
         <v>58</v>
       </c>
       <c r="CK21" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>25</v>
       </c>
       <c r="BM22" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN22" s="1">
         <v>47</v>
@@ -3173,7 +3173,7 @@
         <v>58</v>
       </c>
       <c r="CK22" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:89" ht="135" x14ac:dyDescent="0.25">
@@ -3202,7 +3202,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>90</v>
@@ -3247,7 +3247,7 @@
         <v>73</v>
       </c>
       <c r="BJ23" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BK23" s="1" t="s">
         <v>38</v>
@@ -3256,7 +3256,7 @@
         <v>25</v>
       </c>
       <c r="BM23" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN23" s="1">
         <v>63</v>
@@ -3271,7 +3271,7 @@
         <v>83.2</v>
       </c>
       <c r="CK23" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:89" ht="105" x14ac:dyDescent="0.25">
@@ -3300,7 +3300,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>90</v>
@@ -3336,7 +3336,7 @@
         <v>73</v>
       </c>
       <c r="BJ24" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BK24" s="1" t="s">
         <v>2</v>
@@ -3345,7 +3345,7 @@
         <v>25</v>
       </c>
       <c r="BM24" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN24" s="1">
         <v>156</v>
@@ -3360,7 +3360,7 @@
         <v>672.9</v>
       </c>
       <c r="CK24" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:89" ht="75" x14ac:dyDescent="0.25">
@@ -3413,7 +3413,7 @@
         <v>25</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BN25" s="1">
         <v>56</v>
@@ -3422,7 +3422,7 @@
         <v>58</v>
       </c>
       <c r="CK25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:89" ht="90" x14ac:dyDescent="0.25">
@@ -3451,7 +3451,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>90</v>
@@ -3481,7 +3481,7 @@
         <v>25</v>
       </c>
       <c r="BM26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BN26" s="1">
         <v>31</v>
@@ -3549,7 +3549,7 @@
         <v>25</v>
       </c>
       <c r="BM27" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BN27" s="1">
         <v>29</v>
@@ -3590,7 +3590,7 @@
         <v>22</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>90</v>
@@ -3632,7 +3632,7 @@
         <v>48.7</v>
       </c>
       <c r="BG28" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BI28" s="1" t="s">
         <v>75</v>
@@ -3644,7 +3644,7 @@
         <v>25</v>
       </c>
       <c r="BM28" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BN28" s="1">
         <v>14</v>
@@ -3662,7 +3662,7 @@
         <v>7774</v>
       </c>
       <c r="CK28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:89" ht="120" x14ac:dyDescent="0.25">
@@ -3730,7 +3730,7 @@
         <v>41.3</v>
       </c>
       <c r="BG29" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BI29" s="1" t="s">
         <v>75</v>
@@ -3742,7 +3742,7 @@
         <v>25</v>
       </c>
       <c r="BM29" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BN29" s="1">
         <v>14</v>
@@ -3760,7 +3760,7 @@
         <v>8492</v>
       </c>
       <c r="CK29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:89" ht="105" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
         <v>25</v>
       </c>
       <c r="BM30" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BN30" s="1">
         <v>11</v>
@@ -3911,7 +3911,7 @@
         <v>25</v>
       </c>
       <c r="BM31" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BN31" s="1">
         <v>9</v>
@@ -3955,7 +3955,7 @@
         <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>90</v>
@@ -3997,7 +3997,7 @@
         <v>25</v>
       </c>
       <c r="BM32" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BN32" s="1">
         <v>10</v>
@@ -4041,7 +4041,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>90</v>
@@ -4080,7 +4080,7 @@
         <v>25</v>
       </c>
       <c r="BM33" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BN33" s="1">
         <v>7</v>
@@ -4124,7 +4124,7 @@
         <v>22</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>91</v>
@@ -4163,7 +4163,7 @@
         <v>25</v>
       </c>
       <c r="BM34" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BN34" s="1">
         <v>7</v>
@@ -4207,7 +4207,7 @@
         <v>22</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>90</v>
@@ -4246,7 +4246,7 @@
         <v>25</v>
       </c>
       <c r="BM35" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BN35" s="1">
         <v>5</v>
@@ -4290,7 +4290,7 @@
         <v>22</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>91</v>
@@ -4329,7 +4329,7 @@
         <v>25</v>
       </c>
       <c r="BM36" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BN36" s="1">
         <v>5</v>
@@ -4373,7 +4373,7 @@
         <v>22</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>90</v>
@@ -4430,7 +4430,7 @@
         <v>25</v>
       </c>
       <c r="BM37" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BN37" s="1">
         <v>34</v>
@@ -4445,7 +4445,7 @@
         <v>0.3</v>
       </c>
       <c r="CK37" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:89" ht="225" x14ac:dyDescent="0.25">
@@ -4474,7 +4474,7 @@
         <v>22</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>137</v>
@@ -4524,7 +4524,7 @@
         <v>25</v>
       </c>
       <c r="BM38" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BN38" s="1">
         <v>34</v>
@@ -4539,7 +4539,7 @@
         <v>0.3</v>
       </c>
       <c r="CK38" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:89" ht="225" x14ac:dyDescent="0.25">
@@ -4568,7 +4568,7 @@
         <v>22</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>91</v>
@@ -4618,7 +4618,7 @@
         <v>25</v>
       </c>
       <c r="BM39" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BN39" s="1">
         <v>23</v>
@@ -4633,7 +4633,7 @@
         <v>0.3</v>
       </c>
       <c r="CK39" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>